<commit_message>
move 2023 files and update 2024 files
</commit_message>
<xml_diff>
--- a/data/escapement/prelim-inseason/AUC_DataAnalysisTable_area21-22_2024.xlsx
+++ b/data/escapement/prelim-inseason/AUC_DataAnalysisTable_area21-22_2024.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="AUC_DataAnalysisTable"/>
   </sheets>
   <definedNames>
-    <definedName name="AUC_DataAnalysisTable">'AUC_DataAnalysisTable'!$A$1:$AC$52</definedName>
+    <definedName name="AUC_DataAnalysisTable">'AUC_DataAnalysisTable'!$A$1:$AC$67</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -347,7 +347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC52"/>
+  <dimension ref="A1:AC67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -580,7 +580,7 @@
         <v>1906</v>
       </c>
       <c r="AB2" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC2" s="0" t="inlineStr">
         <is>
@@ -663,7 +663,7 @@
         <v>2</v>
       </c>
       <c r="AB3" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC3" s="0" t="inlineStr">
         <is>
@@ -752,7 +752,7 @@
         <v>35</v>
       </c>
       <c r="AB4" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC4" s="0" t="inlineStr">
         <is>
@@ -823,7 +823,7 @@
         <v>0</v>
       </c>
       <c r="AB5" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC5" s="0" t="inlineStr">
         <is>
@@ -889,7 +889,7 @@
         <v>0</v>
       </c>
       <c r="AB6" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC6" s="0" t="inlineStr">
         <is>
@@ -903,20 +903,20 @@
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>NITINAT RIVER</t>
+          <t>LITTLE NITINAT RIVER</t>
         </is>
       </c>
       <c r="C7" s="1">
-        <v>45504</v>
+        <v>45589</v>
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-37600-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E7" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F7" s="0" t="inlineStr">
@@ -925,19 +925,19 @@
         </is>
       </c>
       <c r="G7" s="0">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="H7" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I7" s="0" t="inlineStr">
         <is>
-          <t>3 - 5 m or to Bottom</t>
+          <t>1 - 3 m</t>
         </is>
       </c>
       <c r="J7" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K7" s="0" t="inlineStr">
@@ -946,17 +946,17 @@
         </is>
       </c>
       <c r="L7" s="0">
-        <v>1</v>
+        <v>380</v>
       </c>
       <c r="N7" s="0">
-        <v>1</v>
+        <v>380</v>
       </c>
       <c r="Q7" s="0">
         <v>0</v>
       </c>
       <c r="T7" s="0" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
       <c r="U7" s="0">
@@ -969,10 +969,10 @@
         <v>1</v>
       </c>
       <c r="X7" s="0">
-        <v>1</v>
+        <v>380</v>
       </c>
       <c r="AB7" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC7" s="0" t="inlineStr">
         <is>
@@ -986,20 +986,20 @@
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>NITINAT RIVER</t>
+          <t>LITTLE NITINAT RIVER</t>
         </is>
       </c>
       <c r="C8" s="1">
-        <v>45504</v>
+        <v>45589</v>
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-37600-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E8" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F8" s="0" t="inlineStr">
@@ -1008,19 +1008,19 @@
         </is>
       </c>
       <c r="G8" s="0">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="H8" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I8" s="0" t="inlineStr">
         <is>
-          <t>3 - 5 m or to Bottom</t>
+          <t>1 - 3 m</t>
         </is>
       </c>
       <c r="J8" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K8" s="0" t="inlineStr">
@@ -1038,7 +1038,7 @@
         <v>0</v>
       </c>
       <c r="AB8" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC8" s="0" t="inlineStr">
         <is>
@@ -1052,20 +1052,20 @@
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>NITINAT RIVER</t>
+          <t>LITTLE NITINAT RIVER</t>
         </is>
       </c>
       <c r="C9" s="1">
-        <v>45504</v>
+        <v>45589</v>
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-37600-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E9" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F9" s="0" t="inlineStr">
@@ -1074,19 +1074,19 @@
         </is>
       </c>
       <c r="G9" s="0">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="H9" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I9" s="0" t="inlineStr">
         <is>
-          <t>3 - 5 m or to Bottom</t>
+          <t>1 - 3 m</t>
         </is>
       </c>
       <c r="J9" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K9" s="0" t="inlineStr">
@@ -1104,7 +1104,7 @@
         <v>0</v>
       </c>
       <c r="AB9" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC9" s="0" t="inlineStr">
         <is>
@@ -1118,76 +1118,64 @@
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>NITINAT RIVER</t>
+          <t>LITTLE NITINAT RIVER</t>
         </is>
       </c>
       <c r="C10" s="1">
-        <v>45504</v>
+        <v>45589</v>
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-37600-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E10" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F10" s="0" t="inlineStr">
         <is>
-          <t>OT</t>
+          <t>PK</t>
         </is>
       </c>
       <c r="G10" s="0">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="H10" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I10" s="0" t="inlineStr">
         <is>
-          <t>3 - 5 m or to Bottom</t>
+          <t>1 - 3 m</t>
         </is>
       </c>
       <c r="J10" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K10" s="0" t="inlineStr">
         <is>
-          <t>Cutthroat</t>
-        </is>
-      </c>
-      <c r="L10" s="0">
-        <v>32</v>
-      </c>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="L10" s="0"/>
       <c r="N10" s="0">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="0">
         <v>0</v>
       </c>
-      <c r="T10" s="0" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="U10" s="0">
-        <v>0.850000023841858</v>
-      </c>
+      <c r="T10" s="0" t="inlineStr"/>
+      <c r="U10" s="0"/>
       <c r="V10" s="0">
         <v>0</v>
       </c>
-      <c r="W10" s="0">
-        <v>0.864864885807037</v>
-      </c>
-      <c r="X10" s="0">
-        <v>44</v>
-      </c>
+      <c r="W10" s="0"/>
+      <c r="X10" s="0"/>
       <c r="AB10" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC10" s="0" t="inlineStr">
         <is>
@@ -1201,46 +1189,46 @@
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>NITINAT RIVER</t>
+          <t>LITTLE NITINAT RIVER</t>
         </is>
       </c>
       <c r="C11" s="1">
-        <v>45504</v>
+        <v>45589</v>
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-37600-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E11" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F11" s="0" t="inlineStr">
         <is>
-          <t>PK</t>
+          <t>SK</t>
         </is>
       </c>
       <c r="G11" s="0">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="H11" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I11" s="0" t="inlineStr">
         <is>
-          <t>3 - 5 m or to Bottom</t>
+          <t>1 - 3 m</t>
         </is>
       </c>
       <c r="J11" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K11" s="0" t="inlineStr">
         <is>
-          <t>Pink</t>
+          <t>Sockeye</t>
         </is>
       </c>
       <c r="N11" s="0">
@@ -1253,7 +1241,7 @@
         <v>0</v>
       </c>
       <c r="AB11" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC11" s="0" t="inlineStr">
         <is>
@@ -1285,7 +1273,7 @@
       </c>
       <c r="F12" s="0" t="inlineStr">
         <is>
-          <t>SK</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="G12" s="0">
@@ -1306,14 +1294,14 @@
       </c>
       <c r="K12" s="0" t="inlineStr">
         <is>
-          <t>Sockeye</t>
+          <t>Chum</t>
         </is>
       </c>
       <c r="L12" s="0">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="N12" s="0">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="Q12" s="0">
         <v>0</v>
@@ -1324,19 +1312,19 @@
         </is>
       </c>
       <c r="U12" s="0">
-        <v>0.850000023841858</v>
+        <v>1</v>
       </c>
       <c r="V12" s="0">
         <v>0</v>
       </c>
       <c r="W12" s="0">
-        <v>0.866666674613953</v>
+        <v>1</v>
       </c>
       <c r="X12" s="0">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="AB12" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC12" s="0" t="inlineStr">
         <is>
@@ -1354,7 +1342,7 @@
         </is>
       </c>
       <c r="C13" s="1">
-        <v>45539</v>
+        <v>45504</v>
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
@@ -1368,11 +1356,11 @@
       </c>
       <c r="F13" s="0" t="inlineStr">
         <is>
-          <t>CM</t>
+          <t>CN</t>
         </is>
       </c>
       <c r="G13" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H13" s="0">
         <v>3</v>
@@ -1384,17 +1372,15 @@
       </c>
       <c r="J13" s="0" t="inlineStr">
         <is>
-          <t>Extremely Low</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K13" s="0" t="inlineStr">
         <is>
-          <t>Chum</t>
-        </is>
-      </c>
-      <c r="L13" s="0">
-        <v>0</v>
-      </c>
+          <t>Chinook</t>
+        </is>
+      </c>
+      <c r="L13" s="0"/>
       <c r="N13" s="0">
         <v>0</v>
       </c>
@@ -1405,7 +1391,7 @@
         <v>0</v>
       </c>
       <c r="AB13" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC13" s="0" t="inlineStr">
         <is>
@@ -1423,7 +1409,7 @@
         </is>
       </c>
       <c r="C14" s="1">
-        <v>45539</v>
+        <v>45504</v>
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
@@ -1437,11 +1423,11 @@
       </c>
       <c r="F14" s="0" t="inlineStr">
         <is>
-          <t>CN</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="G14" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H14" s="0">
         <v>3</v>
@@ -1453,48 +1439,32 @@
       </c>
       <c r="J14" s="0" t="inlineStr">
         <is>
-          <t>Extremely Low</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K14" s="0" t="inlineStr">
         <is>
-          <t>Chinook</t>
-        </is>
-      </c>
-      <c r="L14" s="0">
-        <v>1955</v>
-      </c>
-      <c r="M14" s="0">
-        <v>0</v>
-      </c>
+          <t>Coho</t>
+        </is>
+      </c>
+      <c r="L14" s="0"/>
+      <c r="M14" s="0"/>
       <c r="N14" s="0">
-        <v>1955</v>
-      </c>
-      <c r="O14" s="0">
-        <v>23</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O14" s="0"/>
       <c r="Q14" s="0">
-        <v>23</v>
-      </c>
-      <c r="T14" s="0" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="U14" s="0">
-        <v>0.850000023841858</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T14" s="0" t="inlineStr"/>
+      <c r="U14" s="0"/>
       <c r="V14" s="0">
         <v>0</v>
       </c>
-      <c r="W14" s="0">
-        <v>0.882618486881256</v>
-      </c>
-      <c r="X14" s="0">
-        <v>2606</v>
-      </c>
+      <c r="W14" s="0"/>
+      <c r="X14" s="0"/>
       <c r="AB14" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC14" s="0" t="inlineStr">
         <is>
@@ -1512,7 +1482,7 @@
         </is>
       </c>
       <c r="C15" s="1">
-        <v>45539</v>
+        <v>45504</v>
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
@@ -1526,11 +1496,11 @@
       </c>
       <c r="F15" s="0" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>OT</t>
         </is>
       </c>
       <c r="G15" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H15" s="0">
         <v>3</v>
@@ -1542,48 +1512,44 @@
       </c>
       <c r="J15" s="0" t="inlineStr">
         <is>
-          <t>Extremely Low</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K15" s="0" t="inlineStr">
         <is>
-          <t>Coho</t>
+          <t>Cutthroat</t>
         </is>
       </c>
       <c r="L15" s="0">
-        <v>120</v>
-      </c>
-      <c r="M15" s="0">
-        <v>0</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="M15" s="0"/>
       <c r="N15" s="0">
-        <v>120</v>
-      </c>
-      <c r="O15" s="0">
-        <v>6</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="O15" s="0"/>
       <c r="Q15" s="0">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T15" s="0" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
       <c r="U15" s="0">
-        <v>1</v>
+        <v>0.850000023841858</v>
       </c>
       <c r="V15" s="0">
         <v>0</v>
       </c>
       <c r="W15" s="0">
-        <v>0.967741906642914</v>
+        <v>0.864864885807037</v>
       </c>
       <c r="X15" s="0">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="AB15" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC15" s="0" t="inlineStr">
         <is>
@@ -1601,7 +1567,7 @@
         </is>
       </c>
       <c r="C16" s="1">
-        <v>45539</v>
+        <v>45504</v>
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
@@ -1619,7 +1585,7 @@
         </is>
       </c>
       <c r="G16" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H16" s="0">
         <v>3</v>
@@ -1631,7 +1597,7 @@
       </c>
       <c r="J16" s="0" t="inlineStr">
         <is>
-          <t>Extremely Low</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K16" s="0" t="inlineStr">
@@ -1639,9 +1605,7 @@
           <t>Pink</t>
         </is>
       </c>
-      <c r="L16" s="0">
-        <v>0</v>
-      </c>
+      <c r="L16" s="0"/>
       <c r="N16" s="0">
         <v>0</v>
       </c>
@@ -1652,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="AB16" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC16" s="0" t="inlineStr">
         <is>
@@ -1670,7 +1634,7 @@
         </is>
       </c>
       <c r="C17" s="1">
-        <v>45539</v>
+        <v>45504</v>
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
@@ -1688,7 +1652,7 @@
         </is>
       </c>
       <c r="G17" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H17" s="0">
         <v>3</v>
@@ -1700,7 +1664,7 @@
       </c>
       <c r="J17" s="0" t="inlineStr">
         <is>
-          <t>Extremely Low</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K17" s="0" t="inlineStr">
@@ -1709,36 +1673,34 @@
         </is>
       </c>
       <c r="L17" s="0">
-        <v>230</v>
-      </c>
-      <c r="M17" s="0">
-        <v>0</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="M17" s="0"/>
       <c r="N17" s="0">
-        <v>230</v>
+        <v>65</v>
       </c>
       <c r="Q17" s="0">
         <v>0</v>
       </c>
       <c r="T17" s="0" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
       <c r="U17" s="0">
-        <v>1</v>
+        <v>0.850000023841858</v>
       </c>
       <c r="V17" s="0">
         <v>0</v>
       </c>
       <c r="W17" s="0">
-        <v>0.962343096733093</v>
+        <v>0.866666674613953</v>
       </c>
       <c r="X17" s="0">
-        <v>239</v>
+        <v>88</v>
       </c>
       <c r="AB17" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC17" s="0" t="inlineStr">
         <is>
@@ -1756,7 +1718,7 @@
         </is>
       </c>
       <c r="C18" s="1">
-        <v>45555</v>
+        <v>45539</v>
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
@@ -1774,7 +1736,7 @@
         </is>
       </c>
       <c r="G18" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18" s="0">
         <v>3</v>
@@ -1795,36 +1757,24 @@
         </is>
       </c>
       <c r="L18" s="0">
-        <v>81</v>
-      </c>
-      <c r="M18" s="0">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M18" s="0"/>
       <c r="N18" s="0">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q18" s="0">
         <v>0</v>
       </c>
-      <c r="T18" s="0" t="inlineStr">
-        <is>
-          <t>H</t>
-        </is>
-      </c>
-      <c r="U18" s="0">
-        <v>1</v>
-      </c>
+      <c r="T18" s="0" t="inlineStr"/>
+      <c r="U18" s="0"/>
       <c r="V18" s="0">
         <v>0</v>
       </c>
-      <c r="W18" s="0">
-        <v>0.920454561710358</v>
-      </c>
-      <c r="X18" s="0">
-        <v>88</v>
-      </c>
+      <c r="W18" s="0"/>
+      <c r="X18" s="0"/>
       <c r="AB18" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC18" s="0" t="inlineStr">
         <is>
@@ -1842,7 +1792,7 @@
         </is>
       </c>
       <c r="C19" s="1">
-        <v>45555</v>
+        <v>45539</v>
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
@@ -1860,7 +1810,7 @@
         </is>
       </c>
       <c r="G19" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H19" s="0">
         <v>3</v>
@@ -1881,19 +1831,19 @@
         </is>
       </c>
       <c r="L19" s="0">
-        <v>7293</v>
+        <v>1955</v>
       </c>
       <c r="M19" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N19" s="0">
-        <v>7296</v>
+        <v>1955</v>
       </c>
       <c r="O19" s="0">
-        <v>295</v>
+        <v>23</v>
       </c>
       <c r="Q19" s="0">
-        <v>295</v>
+        <v>23</v>
       </c>
       <c r="T19" s="0" t="inlineStr">
         <is>
@@ -1901,19 +1851,19 @@
         </is>
       </c>
       <c r="U19" s="0">
-        <v>1</v>
+        <v>0.850000023841858</v>
       </c>
       <c r="V19" s="0">
         <v>0</v>
       </c>
       <c r="W19" s="0">
-        <v>0.90293425321579</v>
+        <v>0.882618486881256</v>
       </c>
       <c r="X19" s="0">
-        <v>8077</v>
+        <v>2606</v>
       </c>
       <c r="AB19" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC19" s="0" t="inlineStr">
         <is>
@@ -1931,7 +1881,7 @@
         </is>
       </c>
       <c r="C20" s="1">
-        <v>45555</v>
+        <v>45539</v>
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
@@ -1949,7 +1899,7 @@
         </is>
       </c>
       <c r="G20" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H20" s="0">
         <v>3</v>
@@ -1970,19 +1920,19 @@
         </is>
       </c>
       <c r="L20" s="0">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="M20" s="0">
         <v>0</v>
       </c>
       <c r="N20" s="0">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="O20" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q20" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T20" s="0" t="inlineStr">
         <is>
@@ -1996,13 +1946,13 @@
         <v>0</v>
       </c>
       <c r="W20" s="0">
-        <v>1</v>
+        <v>0.967741906642914</v>
       </c>
       <c r="X20" s="0">
-        <v>7</v>
+        <v>124</v>
       </c>
       <c r="AB20" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC20" s="0" t="inlineStr">
         <is>
@@ -2020,7 +1970,7 @@
         </is>
       </c>
       <c r="C21" s="1">
-        <v>45555</v>
+        <v>45539</v>
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
@@ -2038,7 +1988,7 @@
         </is>
       </c>
       <c r="G21" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21" s="0">
         <v>3</v>
@@ -2058,25 +2008,22 @@
           <t>Pink</t>
         </is>
       </c>
+      <c r="L21" s="0">
+        <v>0</v>
+      </c>
       <c r="N21" s="0">
         <v>0</v>
       </c>
       <c r="Q21" s="0">
         <v>0</v>
       </c>
-      <c r="T21" s="0" t="inlineStr">
-        <is>
-          <t>H</t>
-        </is>
-      </c>
-      <c r="U21" s="0">
-        <v>1</v>
-      </c>
+      <c r="T21" s="0" t="inlineStr"/>
+      <c r="U21" s="0"/>
       <c r="V21" s="0">
         <v>0</v>
       </c>
       <c r="AB21" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC21" s="0" t="inlineStr">
         <is>
@@ -2094,7 +2041,7 @@
         </is>
       </c>
       <c r="C22" s="1">
-        <v>45555</v>
+        <v>45539</v>
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
@@ -2112,7 +2059,7 @@
         </is>
       </c>
       <c r="G22" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H22" s="0">
         <v>3</v>
@@ -2133,17 +2080,15 @@
         </is>
       </c>
       <c r="L22" s="0">
-        <v>155</v>
+        <v>230</v>
       </c>
       <c r="M22" s="0">
         <v>0</v>
       </c>
       <c r="N22" s="0">
-        <v>155</v>
-      </c>
-      <c r="O22" s="0">
-        <v>0</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="O22" s="0"/>
       <c r="Q22" s="0">
         <v>0</v>
       </c>
@@ -2159,13 +2104,13 @@
         <v>0</v>
       </c>
       <c r="W22" s="0">
-        <v>0.950920224189758</v>
+        <v>0.962343096733093</v>
       </c>
       <c r="X22" s="0">
-        <v>163</v>
+        <v>239</v>
       </c>
       <c r="AB22" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC22" s="0" t="inlineStr">
         <is>
@@ -2183,7 +2128,7 @@
         </is>
       </c>
       <c r="C23" s="1">
-        <v>45566</v>
+        <v>45555</v>
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
@@ -2201,7 +2146,7 @@
         </is>
       </c>
       <c r="G23" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H23" s="0">
         <v>3</v>
@@ -2213,7 +2158,7 @@
       </c>
       <c r="J23" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Extremely Low</t>
         </is>
       </c>
       <c r="K23" s="0" t="inlineStr">
@@ -2222,20 +2167,20 @@
         </is>
       </c>
       <c r="L23" s="0">
-        <v>13858</v>
+        <v>81</v>
       </c>
       <c r="M23" s="0">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N23" s="0">
-        <v>13863</v>
+        <v>82</v>
       </c>
       <c r="Q23" s="0">
         <v>0</v>
       </c>
       <c r="T23" s="0" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
       <c r="U23" s="0">
@@ -2245,13 +2190,13 @@
         <v>0</v>
       </c>
       <c r="W23" s="0">
-        <v>0.845360815525055</v>
+        <v>0.920454561710358</v>
       </c>
       <c r="X23" s="0">
-        <v>16393</v>
+        <v>88</v>
       </c>
       <c r="AB23" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC23" s="0" t="inlineStr">
         <is>
@@ -2269,7 +2214,7 @@
         </is>
       </c>
       <c r="C24" s="1">
-        <v>45566</v>
+        <v>45555</v>
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
@@ -2287,7 +2232,7 @@
         </is>
       </c>
       <c r="G24" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H24" s="0">
         <v>3</v>
@@ -2299,7 +2244,7 @@
       </c>
       <c r="J24" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Extremely Low</t>
         </is>
       </c>
       <c r="K24" s="0" t="inlineStr">
@@ -2308,16 +2253,19 @@
         </is>
       </c>
       <c r="L24" s="0">
-        <v>6151</v>
+        <v>7293</v>
       </c>
       <c r="M24" s="0">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="N24" s="0">
-        <v>6173</v>
+        <v>7296</v>
+      </c>
+      <c r="O24" s="0">
+        <v>295</v>
       </c>
       <c r="Q24" s="0">
-        <v>0</v>
+        <v>295</v>
       </c>
       <c r="T24" s="0" t="inlineStr">
         <is>
@@ -2331,13 +2279,13 @@
         <v>0</v>
       </c>
       <c r="W24" s="0">
-        <v>0.84064507484436</v>
+        <v>0.90293425321579</v>
       </c>
       <c r="X24" s="0">
-        <v>7317</v>
+        <v>8077</v>
       </c>
       <c r="AB24" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC24" s="0" t="inlineStr">
         <is>
@@ -2355,7 +2303,7 @@
         </is>
       </c>
       <c r="C25" s="1">
-        <v>45566</v>
+        <v>45555</v>
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
@@ -2373,7 +2321,7 @@
         </is>
       </c>
       <c r="G25" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H25" s="0">
         <v>3</v>
@@ -2385,7 +2333,7 @@
       </c>
       <c r="J25" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Extremely Low</t>
         </is>
       </c>
       <c r="K25" s="0" t="inlineStr">
@@ -2394,20 +2342,23 @@
         </is>
       </c>
       <c r="L25" s="0">
-        <v>195</v>
+        <v>7</v>
+      </c>
+      <c r="M25" s="0">
+        <v>0</v>
       </c>
       <c r="N25" s="0">
-        <v>195</v>
+        <v>7</v>
       </c>
       <c r="O25" s="0">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q25" s="0">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T25" s="0" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
       <c r="U25" s="0">
@@ -2417,13 +2368,13 @@
         <v>0</v>
       </c>
       <c r="W25" s="0">
-        <v>0.840517222881317</v>
+        <v>1</v>
       </c>
       <c r="X25" s="0">
-        <v>232</v>
+        <v>7</v>
       </c>
       <c r="AB25" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC25" s="0" t="inlineStr">
         <is>
@@ -2441,7 +2392,7 @@
         </is>
       </c>
       <c r="C26" s="1">
-        <v>45566</v>
+        <v>45555</v>
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
@@ -2459,7 +2410,7 @@
         </is>
       </c>
       <c r="G26" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H26" s="0">
         <v>3</v>
@@ -2471,7 +2422,7 @@
       </c>
       <c r="J26" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Extremely Low</t>
         </is>
       </c>
       <c r="K26" s="0" t="inlineStr">
@@ -2479,20 +2430,26 @@
           <t>Pink</t>
         </is>
       </c>
-      <c r="L26" s="0">
-        <v>0</v>
-      </c>
+      <c r="L26" s="0"/>
       <c r="N26" s="0">
         <v>0</v>
       </c>
       <c r="Q26" s="0">
         <v>0</v>
       </c>
+      <c r="T26" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U26" s="0">
+        <v>1</v>
+      </c>
       <c r="V26" s="0">
         <v>0</v>
       </c>
       <c r="AB26" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC26" s="0" t="inlineStr">
         <is>
@@ -2510,7 +2467,7 @@
         </is>
       </c>
       <c r="C27" s="1">
-        <v>45566</v>
+        <v>45555</v>
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
@@ -2528,7 +2485,7 @@
         </is>
       </c>
       <c r="G27" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H27" s="0">
         <v>3</v>
@@ -2540,7 +2497,7 @@
       </c>
       <c r="J27" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Extremely Low</t>
         </is>
       </c>
       <c r="K27" s="0" t="inlineStr">
@@ -2549,17 +2506,23 @@
         </is>
       </c>
       <c r="L27" s="0">
-        <v>42</v>
+        <v>155</v>
+      </c>
+      <c r="M27" s="0">
+        <v>0</v>
       </c>
       <c r="N27" s="0">
-        <v>42</v>
+        <v>155</v>
+      </c>
+      <c r="O27" s="0">
+        <v>0</v>
       </c>
       <c r="Q27" s="0">
         <v>0</v>
       </c>
       <c r="T27" s="0" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
       <c r="U27" s="0">
@@ -2569,13 +2532,13 @@
         <v>0</v>
       </c>
       <c r="W27" s="0">
-        <v>0.531645596027374</v>
+        <v>0.950920224189758</v>
       </c>
       <c r="X27" s="0">
-        <v>79</v>
+        <v>163</v>
       </c>
       <c r="AB27" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC27" s="0" t="inlineStr">
         <is>
@@ -2593,7 +2556,7 @@
         </is>
       </c>
       <c r="C28" s="1">
-        <v>45576</v>
+        <v>45566</v>
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
@@ -2616,6 +2579,11 @@
       <c r="H28" s="0">
         <v>3</v>
       </c>
+      <c r="I28" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
       <c r="J28" s="0" t="inlineStr">
         <is>
           <t>Below Norm</t>
@@ -2627,20 +2595,20 @@
         </is>
       </c>
       <c r="L28" s="0">
-        <v>51744</v>
+        <v>13858</v>
       </c>
       <c r="M28" s="0">
-        <v>4168</v>
+        <v>5</v>
       </c>
       <c r="N28" s="0">
-        <v>55912</v>
+        <v>13863</v>
       </c>
       <c r="Q28" s="0">
         <v>0</v>
       </c>
       <c r="T28" s="0" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
       <c r="U28" s="0">
@@ -2650,13 +2618,13 @@
         <v>0</v>
       </c>
       <c r="W28" s="0">
-        <v>0.820278704166412</v>
+        <v>0.845360815525055</v>
       </c>
       <c r="X28" s="0">
-        <v>63081</v>
+        <v>16393</v>
       </c>
       <c r="AB28" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC28" s="0" t="inlineStr">
         <is>
@@ -2674,7 +2642,7 @@
         </is>
       </c>
       <c r="C29" s="1">
-        <v>45576</v>
+        <v>45566</v>
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
@@ -2697,6 +2665,11 @@
       <c r="H29" s="0">
         <v>3</v>
       </c>
+      <c r="I29" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
       <c r="J29" s="0" t="inlineStr">
         <is>
           <t>Below Norm</t>
@@ -2708,23 +2681,21 @@
         </is>
       </c>
       <c r="L29" s="0">
-        <v>3049</v>
+        <v>6151</v>
       </c>
       <c r="M29" s="0">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="N29" s="0">
-        <v>3109</v>
-      </c>
-      <c r="O29" s="0">
-        <v>1</v>
-      </c>
+        <v>6173</v>
+      </c>
+      <c r="O29" s="0"/>
       <c r="Q29" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T29" s="0" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
       <c r="U29" s="0">
@@ -2734,13 +2705,13 @@
         <v>0</v>
       </c>
       <c r="W29" s="0">
-        <v>0.861786305904388</v>
+        <v>0.84064507484436</v>
       </c>
       <c r="X29" s="0">
-        <v>3538</v>
+        <v>7317</v>
       </c>
       <c r="AB29" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC29" s="0" t="inlineStr">
         <is>
@@ -2758,7 +2729,7 @@
         </is>
       </c>
       <c r="C30" s="1">
-        <v>45576</v>
+        <v>45566</v>
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
@@ -2781,6 +2752,11 @@
       <c r="H30" s="0">
         <v>3</v>
       </c>
+      <c r="I30" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
       <c r="J30" s="0" t="inlineStr">
         <is>
           <t>Below Norm</t>
@@ -2792,20 +2768,20 @@
         </is>
       </c>
       <c r="L30" s="0">
-        <v>1494</v>
+        <v>195</v>
       </c>
       <c r="N30" s="0">
-        <v>1494</v>
+        <v>195</v>
       </c>
       <c r="O30" s="0">
-        <v>173</v>
+        <v>20</v>
       </c>
       <c r="Q30" s="0">
-        <v>173</v>
+        <v>20</v>
       </c>
       <c r="T30" s="0" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
       <c r="U30" s="0">
@@ -2815,13 +2791,13 @@
         <v>0</v>
       </c>
       <c r="W30" s="0">
-        <v>0.862586617469788</v>
+        <v>0.840517222881317</v>
       </c>
       <c r="X30" s="0">
-        <v>1732</v>
+        <v>232</v>
       </c>
       <c r="AB30" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC30" s="0" t="inlineStr">
         <is>
@@ -2839,7 +2815,7 @@
         </is>
       </c>
       <c r="C31" s="1">
-        <v>45576</v>
+        <v>45566</v>
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
@@ -2862,6 +2838,11 @@
       <c r="H31" s="0">
         <v>3</v>
       </c>
+      <c r="I31" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
       <c r="J31" s="0" t="inlineStr">
         <is>
           <t>Below Norm</t>
@@ -2872,6 +2853,9 @@
           <t>Pink</t>
         </is>
       </c>
+      <c r="L31" s="0">
+        <v>0</v>
+      </c>
       <c r="N31" s="0">
         <v>0</v>
       </c>
@@ -2882,7 +2866,7 @@
         <v>0</v>
       </c>
       <c r="AB31" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC31" s="0" t="inlineStr">
         <is>
@@ -2900,7 +2884,7 @@
         </is>
       </c>
       <c r="C32" s="1">
-        <v>45576</v>
+        <v>45566</v>
       </c>
       <c r="D32" s="0" t="inlineStr">
         <is>
@@ -2923,6 +2907,11 @@
       <c r="H32" s="0">
         <v>3</v>
       </c>
+      <c r="I32" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
       <c r="J32" s="0" t="inlineStr">
         <is>
           <t>Below Norm</t>
@@ -2934,20 +2923,18 @@
         </is>
       </c>
       <c r="L32" s="0">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="N32" s="0">
-        <v>64</v>
-      </c>
-      <c r="O32" s="0">
-        <v>1</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="O32" s="0"/>
       <c r="Q32" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T32" s="0" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
       <c r="U32" s="0">
@@ -2957,13 +2944,13 @@
         <v>0</v>
       </c>
       <c r="W32" s="0">
-        <v>0.853333353996277</v>
+        <v>0.531645596027374</v>
       </c>
       <c r="X32" s="0">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="AB32" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC32" s="0" t="inlineStr">
         <is>
@@ -2981,7 +2968,7 @@
         </is>
       </c>
       <c r="C33" s="1">
-        <v>45589</v>
+        <v>45576</v>
       </c>
       <c r="D33" s="0" t="inlineStr">
         <is>
@@ -2999,19 +2986,15 @@
         </is>
       </c>
       <c r="G33" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H33" s="0">
         <v>3</v>
       </c>
-      <c r="I33" s="0" t="inlineStr">
-        <is>
-          <t>1 - 3 m</t>
-        </is>
-      </c>
+      <c r="I33" s="0" t="inlineStr"/>
       <c r="J33" s="0" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K33" s="0" t="inlineStr">
@@ -3020,20 +3003,20 @@
         </is>
       </c>
       <c r="L33" s="0">
-        <v>128669</v>
+        <v>51744</v>
       </c>
       <c r="M33" s="0">
-        <v>680</v>
+        <v>4168</v>
       </c>
       <c r="N33" s="0">
-        <v>129349</v>
+        <v>55912</v>
       </c>
       <c r="Q33" s="0">
         <v>0</v>
       </c>
       <c r="T33" s="0" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
       <c r="U33" s="0">
@@ -3043,13 +3026,13 @@
         <v>0</v>
       </c>
       <c r="W33" s="0">
-        <v>0.936926126480103</v>
+        <v>0.820278704166412</v>
       </c>
       <c r="X33" s="0">
-        <v>137331</v>
+        <v>63081</v>
       </c>
       <c r="AB33" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC33" s="0" t="inlineStr">
         <is>
@@ -3067,7 +3050,7 @@
         </is>
       </c>
       <c r="C34" s="1">
-        <v>45589</v>
+        <v>45576</v>
       </c>
       <c r="D34" s="0" t="inlineStr">
         <is>
@@ -3085,19 +3068,15 @@
         </is>
       </c>
       <c r="G34" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H34" s="0">
         <v>3</v>
       </c>
-      <c r="I34" s="0" t="inlineStr">
-        <is>
-          <t>1 - 3 m</t>
-        </is>
-      </c>
+      <c r="I34" s="0" t="inlineStr"/>
       <c r="J34" s="0" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K34" s="0" t="inlineStr">
@@ -3106,10 +3085,13 @@
         </is>
       </c>
       <c r="L34" s="0">
-        <v>39</v>
+        <v>3049</v>
+      </c>
+      <c r="M34" s="0">
+        <v>60</v>
       </c>
       <c r="N34" s="0">
-        <v>39</v>
+        <v>3109</v>
       </c>
       <c r="O34" s="0">
         <v>1</v>
@@ -3119,7 +3101,7 @@
       </c>
       <c r="T34" s="0" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
       <c r="U34" s="0">
@@ -3129,13 +3111,13 @@
         <v>0</v>
       </c>
       <c r="W34" s="0">
-        <v>0.847826063632965</v>
+        <v>0.861786305904388</v>
       </c>
       <c r="X34" s="0">
-        <v>46</v>
+        <v>3538</v>
       </c>
       <c r="AB34" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC34" s="0" t="inlineStr">
         <is>
@@ -3153,7 +3135,7 @@
         </is>
       </c>
       <c r="C35" s="1">
-        <v>45589</v>
+        <v>45576</v>
       </c>
       <c r="D35" s="0" t="inlineStr">
         <is>
@@ -3171,19 +3153,15 @@
         </is>
       </c>
       <c r="G35" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H35" s="0">
         <v>3</v>
       </c>
-      <c r="I35" s="0" t="inlineStr">
-        <is>
-          <t>1 - 3 m</t>
-        </is>
-      </c>
+      <c r="I35" s="0" t="inlineStr"/>
       <c r="J35" s="0" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K35" s="0" t="inlineStr">
@@ -3192,20 +3170,20 @@
         </is>
       </c>
       <c r="L35" s="0">
-        <v>21</v>
+        <v>1494</v>
       </c>
       <c r="N35" s="0">
-        <v>21</v>
+        <v>1494</v>
       </c>
       <c r="O35" s="0">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="Q35" s="0">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="T35" s="0" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>H</t>
         </is>
       </c>
       <c r="U35" s="0">
@@ -3215,13 +3193,13 @@
         <v>0</v>
       </c>
       <c r="W35" s="0">
-        <v>0.91304349899292</v>
+        <v>0.862586617469788</v>
       </c>
       <c r="X35" s="0">
-        <v>23</v>
+        <v>1732</v>
       </c>
       <c r="AB35" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC35" s="0" t="inlineStr">
         <is>
@@ -3239,7 +3217,7 @@
         </is>
       </c>
       <c r="C36" s="1">
-        <v>45589</v>
+        <v>45576</v>
       </c>
       <c r="D36" s="0" t="inlineStr">
         <is>
@@ -3257,19 +3235,15 @@
         </is>
       </c>
       <c r="G36" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H36" s="0">
         <v>3</v>
       </c>
-      <c r="I36" s="0" t="inlineStr">
-        <is>
-          <t>1 - 3 m</t>
-        </is>
-      </c>
+      <c r="I36" s="0" t="inlineStr"/>
       <c r="J36" s="0" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K36" s="0" t="inlineStr">
@@ -3287,7 +3261,7 @@
         <v>0</v>
       </c>
       <c r="AB36" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC36" s="0" t="inlineStr">
         <is>
@@ -3305,7 +3279,7 @@
         </is>
       </c>
       <c r="C37" s="1">
-        <v>45589</v>
+        <v>45576</v>
       </c>
       <c r="D37" s="0" t="inlineStr">
         <is>
@@ -3323,19 +3297,15 @@
         </is>
       </c>
       <c r="G37" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H37" s="0">
         <v>3</v>
       </c>
-      <c r="I37" s="0" t="inlineStr">
-        <is>
-          <t>1 - 3 m</t>
-        </is>
-      </c>
+      <c r="I37" s="0" t="inlineStr"/>
       <c r="J37" s="0" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K37" s="0" t="inlineStr">
@@ -3344,17 +3314,20 @@
         </is>
       </c>
       <c r="L37" s="0">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="N37" s="0">
-        <v>2</v>
+        <v>64</v>
+      </c>
+      <c r="O37" s="0">
+        <v>1</v>
       </c>
       <c r="Q37" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T37" s="0" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>H</t>
         </is>
       </c>
       <c r="U37" s="0">
@@ -3364,13 +3337,13 @@
         <v>0</v>
       </c>
       <c r="W37" s="0">
-        <v>1</v>
+        <v>0.853333353996277</v>
       </c>
       <c r="X37" s="0">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="AB37" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC37" s="0" t="inlineStr">
         <is>
@@ -3388,7 +3361,7 @@
         </is>
       </c>
       <c r="C38" s="1">
-        <v>45603</v>
+        <v>45588</v>
       </c>
       <c r="D38" s="0" t="inlineStr">
         <is>
@@ -3397,7 +3370,7 @@
       </c>
       <c r="E38" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F38" s="0" t="inlineStr">
@@ -3406,10 +3379,10 @@
         </is>
       </c>
       <c r="G38" s="0">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="H38" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I38" s="0" t="inlineStr">
         <is>
@@ -3418,7 +3391,7 @@
       </c>
       <c r="J38" s="0" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K38" s="0" t="inlineStr">
@@ -3427,20 +3400,20 @@
         </is>
       </c>
       <c r="L38" s="0">
-        <v>493</v>
+        <v>99250</v>
       </c>
       <c r="M38" s="0">
-        <v>2388</v>
+        <v>3000</v>
       </c>
       <c r="N38" s="0">
-        <v>2881</v>
+        <v>102250</v>
       </c>
       <c r="Q38" s="0">
         <v>0</v>
       </c>
       <c r="T38" s="0" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
       <c r="U38" s="0">
@@ -3450,13 +3423,13 @@
         <v>0</v>
       </c>
       <c r="W38" s="0">
-        <v>0.767912745475769</v>
+        <v>1</v>
       </c>
       <c r="X38" s="0">
-        <v>642</v>
+        <v>99250</v>
       </c>
       <c r="AB38" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC38" s="0" t="inlineStr">
         <is>
@@ -3474,7 +3447,7 @@
         </is>
       </c>
       <c r="C39" s="1">
-        <v>45603</v>
+        <v>45588</v>
       </c>
       <c r="D39" s="0" t="inlineStr">
         <is>
@@ -3483,7 +3456,7 @@
       </c>
       <c r="E39" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F39" s="0" t="inlineStr">
@@ -3492,10 +3465,10 @@
         </is>
       </c>
       <c r="G39" s="0">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="H39" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I39" s="0" t="inlineStr">
         <is>
@@ -3504,7 +3477,7 @@
       </c>
       <c r="J39" s="0" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K39" s="0" t="inlineStr">
@@ -3512,40 +3485,24 @@
           <t>Chinook</t>
         </is>
       </c>
-      <c r="L39" s="0">
-        <v>4</v>
-      </c>
-      <c r="M39" s="0">
-        <v>0</v>
-      </c>
+      <c r="L39" s="0"/>
+      <c r="M39" s="0"/>
       <c r="N39" s="0">
-        <v>4</v>
-      </c>
-      <c r="O39" s="0">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O39" s="0"/>
       <c r="Q39" s="0">
         <v>0</v>
       </c>
-      <c r="T39" s="0" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="U39" s="0">
-        <v>1</v>
-      </c>
+      <c r="T39" s="0" t="inlineStr"/>
+      <c r="U39" s="0"/>
       <c r="V39" s="0">
         <v>0</v>
       </c>
-      <c r="W39" s="0">
-        <v>0.800000011920929</v>
-      </c>
-      <c r="X39" s="0">
-        <v>5</v>
-      </c>
+      <c r="W39" s="0"/>
+      <c r="X39" s="0"/>
       <c r="AB39" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC39" s="0" t="inlineStr">
         <is>
@@ -3563,7 +3520,7 @@
         </is>
       </c>
       <c r="C40" s="1">
-        <v>45603</v>
+        <v>45588</v>
       </c>
       <c r="D40" s="0" t="inlineStr">
         <is>
@@ -3572,7 +3529,7 @@
       </c>
       <c r="E40" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F40" s="0" t="inlineStr">
@@ -3581,10 +3538,10 @@
         </is>
       </c>
       <c r="G40" s="0">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="H40" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I40" s="0" t="inlineStr">
         <is>
@@ -3593,7 +3550,7 @@
       </c>
       <c r="J40" s="0" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K40" s="0" t="inlineStr">
@@ -3601,40 +3558,24 @@
           <t>Coho</t>
         </is>
       </c>
-      <c r="L40" s="0">
-        <v>1302</v>
-      </c>
-      <c r="M40" s="0">
-        <v>8</v>
-      </c>
+      <c r="L40" s="0"/>
+      <c r="M40" s="0"/>
       <c r="N40" s="0">
-        <v>1310</v>
-      </c>
-      <c r="O40" s="0">
-        <v>148</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O40" s="0"/>
       <c r="Q40" s="0">
-        <v>148</v>
-      </c>
-      <c r="T40" s="0" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="U40" s="0">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="T40" s="0" t="inlineStr"/>
+      <c r="U40" s="0"/>
       <c r="V40" s="0">
         <v>0</v>
       </c>
-      <c r="W40" s="0">
-        <v>0.810709834098816</v>
-      </c>
-      <c r="X40" s="0">
-        <v>1606</v>
-      </c>
+      <c r="W40" s="0"/>
+      <c r="X40" s="0"/>
       <c r="AB40" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC40" s="0" t="inlineStr">
         <is>
@@ -3652,7 +3593,7 @@
         </is>
       </c>
       <c r="C41" s="1">
-        <v>45603</v>
+        <v>45588</v>
       </c>
       <c r="D41" s="0" t="inlineStr">
         <is>
@@ -3661,7 +3602,7 @@
       </c>
       <c r="E41" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F41" s="0" t="inlineStr">
@@ -3670,10 +3611,10 @@
         </is>
       </c>
       <c r="G41" s="0">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="H41" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I41" s="0" t="inlineStr">
         <is>
@@ -3682,7 +3623,7 @@
       </c>
       <c r="J41" s="0" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K41" s="0" t="inlineStr">
@@ -3700,7 +3641,7 @@
         <v>0</v>
       </c>
       <c r="AB41" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC41" s="0" t="inlineStr">
         <is>
@@ -3718,7 +3659,7 @@
         </is>
       </c>
       <c r="C42" s="1">
-        <v>45603</v>
+        <v>45588</v>
       </c>
       <c r="D42" s="0" t="inlineStr">
         <is>
@@ -3727,7 +3668,7 @@
       </c>
       <c r="E42" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F42" s="0" t="inlineStr">
@@ -3736,10 +3677,10 @@
         </is>
       </c>
       <c r="G42" s="0">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="H42" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I42" s="0" t="inlineStr">
         <is>
@@ -3748,7 +3689,7 @@
       </c>
       <c r="J42" s="0" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K42" s="0" t="inlineStr">
@@ -3756,17 +3697,22 @@
           <t>Sockeye</t>
         </is>
       </c>
+      <c r="L42" s="0"/>
       <c r="N42" s="0">
         <v>0</v>
       </c>
       <c r="Q42" s="0">
         <v>0</v>
       </c>
+      <c r="T42" s="0" t="inlineStr"/>
+      <c r="U42" s="0"/>
       <c r="V42" s="0">
         <v>0</v>
       </c>
+      <c r="W42" s="0"/>
+      <c r="X42" s="0"/>
       <c r="AB42" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC42" s="0" t="inlineStr">
         <is>
@@ -3784,7 +3730,7 @@
         </is>
       </c>
       <c r="C43" s="1">
-        <v>45609</v>
+        <v>45589</v>
       </c>
       <c r="D43" s="0" t="inlineStr">
         <is>
@@ -3807,9 +3753,14 @@
       <c r="H43" s="0">
         <v>3</v>
       </c>
+      <c r="I43" s="0" t="inlineStr">
+        <is>
+          <t>1 - 3 m</t>
+        </is>
+      </c>
       <c r="J43" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Flood</t>
         </is>
       </c>
       <c r="K43" s="0" t="inlineStr">
@@ -3818,25 +3769,36 @@
         </is>
       </c>
       <c r="L43" s="0">
-        <v>59</v>
+        <v>128669</v>
       </c>
       <c r="M43" s="0">
-        <v>0</v>
+        <v>680</v>
       </c>
       <c r="N43" s="0">
-        <v>59</v>
+        <v>129349</v>
       </c>
       <c r="Q43" s="0">
         <v>0</v>
       </c>
+      <c r="T43" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U43" s="0">
+        <v>1</v>
+      </c>
       <c r="V43" s="0">
         <v>0</v>
       </c>
       <c r="W43" s="0">
-        <v>0.830985903739929</v>
+        <v>0.936926126480103</v>
+      </c>
+      <c r="X43" s="0">
+        <v>137331</v>
       </c>
       <c r="AB43" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC43" s="0" t="inlineStr">
         <is>
@@ -3854,7 +3816,7 @@
         </is>
       </c>
       <c r="C44" s="1">
-        <v>45609</v>
+        <v>45589</v>
       </c>
       <c r="D44" s="0" t="inlineStr">
         <is>
@@ -3877,9 +3839,14 @@
       <c r="H44" s="0">
         <v>3</v>
       </c>
+      <c r="I44" s="0" t="inlineStr">
+        <is>
+          <t>1 - 3 m</t>
+        </is>
+      </c>
       <c r="J44" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Flood</t>
         </is>
       </c>
       <c r="K44" s="0" t="inlineStr">
@@ -3888,28 +3855,37 @@
         </is>
       </c>
       <c r="L44" s="0">
-        <v>4</v>
-      </c>
-      <c r="M44" s="0">
-        <v>0</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="M44" s="0"/>
       <c r="N44" s="0">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="O44" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q44" s="0">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="T44" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U44" s="0">
+        <v>1</v>
       </c>
       <c r="V44" s="0">
         <v>0</v>
       </c>
       <c r="W44" s="0">
-        <v>0.800000011920929</v>
+        <v>0.847826063632965</v>
+      </c>
+      <c r="X44" s="0">
+        <v>46</v>
       </c>
       <c r="AB44" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC44" s="0" t="inlineStr">
         <is>
@@ -3927,7 +3903,7 @@
         </is>
       </c>
       <c r="C45" s="1">
-        <v>45609</v>
+        <v>45589</v>
       </c>
       <c r="D45" s="0" t="inlineStr">
         <is>
@@ -3950,9 +3926,14 @@
       <c r="H45" s="0">
         <v>3</v>
       </c>
+      <c r="I45" s="0" t="inlineStr">
+        <is>
+          <t>1 - 3 m</t>
+        </is>
+      </c>
       <c r="J45" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Flood</t>
         </is>
       </c>
       <c r="K45" s="0" t="inlineStr">
@@ -3961,28 +3942,37 @@
         </is>
       </c>
       <c r="L45" s="0">
-        <v>626</v>
-      </c>
-      <c r="M45" s="0">
+        <v>21</v>
+      </c>
+      <c r="M45" s="0"/>
+      <c r="N45" s="0">
+        <v>21</v>
+      </c>
+      <c r="O45" s="0">
+        <v>4</v>
+      </c>
+      <c r="Q45" s="0">
+        <v>4</v>
+      </c>
+      <c r="T45" s="0" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="U45" s="0">
         <v>1</v>
       </c>
-      <c r="N45" s="0">
-        <v>627</v>
-      </c>
-      <c r="O45" s="0">
-        <v>100</v>
-      </c>
-      <c r="Q45" s="0">
-        <v>100</v>
-      </c>
       <c r="V45" s="0">
         <v>0</v>
       </c>
       <c r="W45" s="0">
-        <v>1</v>
+        <v>0.91304349899292</v>
+      </c>
+      <c r="X45" s="0">
+        <v>23</v>
       </c>
       <c r="AB45" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC45" s="0" t="inlineStr">
         <is>
@@ -4000,7 +3990,7 @@
         </is>
       </c>
       <c r="C46" s="1">
-        <v>45609</v>
+        <v>45589</v>
       </c>
       <c r="D46" s="0" t="inlineStr">
         <is>
@@ -4023,9 +4013,14 @@
       <c r="H46" s="0">
         <v>3</v>
       </c>
+      <c r="I46" s="0" t="inlineStr">
+        <is>
+          <t>1 - 3 m</t>
+        </is>
+      </c>
       <c r="J46" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Flood</t>
         </is>
       </c>
       <c r="K46" s="0" t="inlineStr">
@@ -4043,7 +4038,7 @@
         <v>0</v>
       </c>
       <c r="AB46" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC46" s="0" t="inlineStr">
         <is>
@@ -4061,7 +4056,7 @@
         </is>
       </c>
       <c r="C47" s="1">
-        <v>45609</v>
+        <v>45589</v>
       </c>
       <c r="D47" s="0" t="inlineStr">
         <is>
@@ -4084,9 +4079,14 @@
       <c r="H47" s="0">
         <v>3</v>
       </c>
+      <c r="I47" s="0" t="inlineStr">
+        <is>
+          <t>1 - 3 m</t>
+        </is>
+      </c>
       <c r="J47" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Flood</t>
         </is>
       </c>
       <c r="K47" s="0" t="inlineStr">
@@ -4094,17 +4094,34 @@
           <t>Sockeye</t>
         </is>
       </c>
+      <c r="L47" s="0">
+        <v>2</v>
+      </c>
       <c r="N47" s="0">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q47" s="0">
         <v>0</v>
       </c>
+      <c r="T47" s="0" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="U47" s="0">
+        <v>1</v>
+      </c>
       <c r="V47" s="0">
         <v>0</v>
       </c>
+      <c r="W47" s="0">
+        <v>1</v>
+      </c>
+      <c r="X47" s="0">
+        <v>2</v>
+      </c>
       <c r="AB47" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC47" s="0" t="inlineStr">
         <is>
@@ -4118,15 +4135,15 @@
       </c>
       <c r="B48" s="0" t="inlineStr">
         <is>
-          <t>WORTHLESS CREEK</t>
+          <t>NITINAT RIVER</t>
         </is>
       </c>
       <c r="C48" s="1">
-        <v>45597</v>
+        <v>45603</v>
       </c>
       <c r="D48" s="0" t="inlineStr">
         <is>
-          <t>930-071700-44200-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E48" s="0" t="inlineStr">
@@ -4140,19 +4157,19 @@
         </is>
       </c>
       <c r="G48" s="0">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="H48" s="0">
         <v>3</v>
       </c>
       <c r="I48" s="0" t="inlineStr">
         <is>
-          <t>3 - 5 m or to Bottom</t>
+          <t>1 - 3 m</t>
         </is>
       </c>
       <c r="J48" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Flood</t>
         </is>
       </c>
       <c r="K48" s="0" t="inlineStr">
@@ -4161,25 +4178,36 @@
         </is>
       </c>
       <c r="L48" s="0">
-        <v>27</v>
+        <v>493</v>
       </c>
       <c r="M48" s="0">
-        <v>186</v>
+        <v>2388</v>
       </c>
       <c r="N48" s="0">
-        <v>213</v>
+        <v>2881</v>
       </c>
       <c r="Q48" s="0">
         <v>0</v>
       </c>
+      <c r="T48" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U48" s="0">
+        <v>1</v>
+      </c>
       <c r="V48" s="0">
         <v>0</v>
       </c>
       <c r="W48" s="0">
-        <v>0.899999976158142</v>
+        <v>0.767912745475769</v>
+      </c>
+      <c r="X48" s="0">
+        <v>642</v>
       </c>
       <c r="AB48" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC48" s="0" t="inlineStr">
         <is>
@@ -4193,15 +4221,15 @@
       </c>
       <c r="B49" s="0" t="inlineStr">
         <is>
-          <t>WORTHLESS CREEK</t>
+          <t>NITINAT RIVER</t>
         </is>
       </c>
       <c r="C49" s="1">
-        <v>45597</v>
+        <v>45603</v>
       </c>
       <c r="D49" s="0" t="inlineStr">
         <is>
-          <t>930-071700-44200-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E49" s="0" t="inlineStr">
@@ -4215,19 +4243,19 @@
         </is>
       </c>
       <c r="G49" s="0">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="H49" s="0">
         <v>3</v>
       </c>
       <c r="I49" s="0" t="inlineStr">
         <is>
-          <t>3 - 5 m or to Bottom</t>
+          <t>1 - 3 m</t>
         </is>
       </c>
       <c r="J49" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Flood</t>
         </is>
       </c>
       <c r="K49" s="0" t="inlineStr">
@@ -4235,17 +4263,40 @@
           <t>Chinook</t>
         </is>
       </c>
+      <c r="L49" s="0">
+        <v>4</v>
+      </c>
+      <c r="M49" s="0">
+        <v>0</v>
+      </c>
       <c r="N49" s="0">
+        <v>4</v>
+      </c>
+      <c r="O49" s="0">
         <v>0</v>
       </c>
       <c r="Q49" s="0">
         <v>0</v>
       </c>
+      <c r="T49" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U49" s="0">
+        <v>1</v>
+      </c>
       <c r="V49" s="0">
         <v>0</v>
       </c>
+      <c r="W49" s="0">
+        <v>0.800000011920929</v>
+      </c>
+      <c r="X49" s="0">
+        <v>5</v>
+      </c>
       <c r="AB49" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC49" s="0" t="inlineStr">
         <is>
@@ -4259,15 +4310,15 @@
       </c>
       <c r="B50" s="0" t="inlineStr">
         <is>
-          <t>WORTHLESS CREEK</t>
+          <t>NITINAT RIVER</t>
         </is>
       </c>
       <c r="C50" s="1">
-        <v>45597</v>
+        <v>45603</v>
       </c>
       <c r="D50" s="0" t="inlineStr">
         <is>
-          <t>930-071700-44200-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E50" s="0" t="inlineStr">
@@ -4281,19 +4332,19 @@
         </is>
       </c>
       <c r="G50" s="0">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="H50" s="0">
         <v>3</v>
       </c>
       <c r="I50" s="0" t="inlineStr">
         <is>
-          <t>3 - 5 m or to Bottom</t>
+          <t>1 - 3 m</t>
         </is>
       </c>
       <c r="J50" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Flood</t>
         </is>
       </c>
       <c r="K50" s="0" t="inlineStr">
@@ -4302,28 +4353,39 @@
         </is>
       </c>
       <c r="L50" s="0">
-        <v>36</v>
+        <v>1302</v>
       </c>
       <c r="M50" s="0">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N50" s="0">
-        <v>36</v>
+        <v>1310</v>
       </c>
       <c r="O50" s="0">
-        <v>8</v>
+        <v>148</v>
       </c>
       <c r="Q50" s="0">
-        <v>8</v>
+        <v>148</v>
+      </c>
+      <c r="T50" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U50" s="0">
+        <v>1</v>
       </c>
       <c r="V50" s="0">
         <v>0</v>
       </c>
       <c r="W50" s="0">
-        <v>0.899999976158142</v>
+        <v>0.810709834098816</v>
+      </c>
+      <c r="X50" s="0">
+        <v>1606</v>
       </c>
       <c r="AB50" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC50" s="0" t="inlineStr">
         <is>
@@ -4337,15 +4399,15 @@
       </c>
       <c r="B51" s="0" t="inlineStr">
         <is>
-          <t>WORTHLESS CREEK</t>
+          <t>NITINAT RIVER</t>
         </is>
       </c>
       <c r="C51" s="1">
-        <v>45597</v>
+        <v>45603</v>
       </c>
       <c r="D51" s="0" t="inlineStr">
         <is>
-          <t>930-071700-44200-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E51" s="0" t="inlineStr">
@@ -4359,19 +4421,19 @@
         </is>
       </c>
       <c r="G51" s="0">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="H51" s="0">
         <v>3</v>
       </c>
       <c r="I51" s="0" t="inlineStr">
         <is>
-          <t>3 - 5 m or to Bottom</t>
+          <t>1 - 3 m</t>
         </is>
       </c>
       <c r="J51" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Flood</t>
         </is>
       </c>
       <c r="K51" s="0" t="inlineStr">
@@ -4389,7 +4451,7 @@
         <v>0</v>
       </c>
       <c r="AB51" s="1">
-        <v>45624.3850810185</v>
+        <v>45624.412349537</v>
       </c>
       <c r="AC51" s="0" t="inlineStr">
         <is>
@@ -4403,15 +4465,15 @@
       </c>
       <c r="B52" s="0" t="inlineStr">
         <is>
-          <t>WORTHLESS CREEK</t>
+          <t>NITINAT RIVER</t>
         </is>
       </c>
       <c r="C52" s="1">
-        <v>45597</v>
+        <v>45603</v>
       </c>
       <c r="D52" s="0" t="inlineStr">
         <is>
-          <t>930-071700-44200-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E52" s="0" t="inlineStr">
@@ -4425,39 +4487,1080 @@
         </is>
       </c>
       <c r="G52" s="0">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="H52" s="0">
         <v>3</v>
       </c>
       <c r="I52" s="0" t="inlineStr">
         <is>
+          <t>1 - 3 m</t>
+        </is>
+      </c>
+      <c r="J52" s="0" t="inlineStr">
+        <is>
+          <t>Flood</t>
+        </is>
+      </c>
+      <c r="K52" s="0" t="inlineStr">
+        <is>
+          <t>Sockeye</t>
+        </is>
+      </c>
+      <c r="N52" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="0">
+        <v>0</v>
+      </c>
+      <c r="V52" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB52" s="1">
+        <v>45624.412349537</v>
+      </c>
+      <c r="AC52" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="53">
+      <c r="A53" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B53" s="0" t="inlineStr">
+        <is>
+          <t>NITINAT RIVER</t>
+        </is>
+      </c>
+      <c r="C53" s="1">
+        <v>45609</v>
+      </c>
+      <c r="D53" s="0" t="inlineStr">
+        <is>
+          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E53" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F53" s="0" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="G53" s="0">
+        <v>8</v>
+      </c>
+      <c r="H53" s="0">
+        <v>3</v>
+      </c>
+      <c r="I53" s="0" t="inlineStr"/>
+      <c r="J53" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K53" s="0" t="inlineStr">
+        <is>
+          <t>Chum</t>
+        </is>
+      </c>
+      <c r="L53" s="0">
+        <v>59</v>
+      </c>
+      <c r="M53" s="0">
+        <v>0</v>
+      </c>
+      <c r="N53" s="0">
+        <v>59</v>
+      </c>
+      <c r="Q53" s="0">
+        <v>0</v>
+      </c>
+      <c r="V53" s="0">
+        <v>0</v>
+      </c>
+      <c r="W53" s="0">
+        <v>0.830985903739929</v>
+      </c>
+      <c r="AB53" s="1">
+        <v>45624.412349537</v>
+      </c>
+      <c r="AC53" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="54">
+      <c r="A54" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B54" s="0" t="inlineStr">
+        <is>
+          <t>NITINAT RIVER</t>
+        </is>
+      </c>
+      <c r="C54" s="1">
+        <v>45609</v>
+      </c>
+      <c r="D54" s="0" t="inlineStr">
+        <is>
+          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E54" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F54" s="0" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G54" s="0">
+        <v>8</v>
+      </c>
+      <c r="H54" s="0">
+        <v>3</v>
+      </c>
+      <c r="I54" s="0" t="inlineStr"/>
+      <c r="J54" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K54" s="0" t="inlineStr">
+        <is>
+          <t>Chinook</t>
+        </is>
+      </c>
+      <c r="L54" s="0">
+        <v>4</v>
+      </c>
+      <c r="M54" s="0">
+        <v>0</v>
+      </c>
+      <c r="N54" s="0">
+        <v>4</v>
+      </c>
+      <c r="O54" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="0">
+        <v>0</v>
+      </c>
+      <c r="V54" s="0">
+        <v>0</v>
+      </c>
+      <c r="W54" s="0">
+        <v>0.800000011920929</v>
+      </c>
+      <c r="AB54" s="1">
+        <v>45624.412349537</v>
+      </c>
+      <c r="AC54" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="55">
+      <c r="A55" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B55" s="0" t="inlineStr">
+        <is>
+          <t>NITINAT RIVER</t>
+        </is>
+      </c>
+      <c r="C55" s="1">
+        <v>45609</v>
+      </c>
+      <c r="D55" s="0" t="inlineStr">
+        <is>
+          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E55" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F55" s="0" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="G55" s="0">
+        <v>8</v>
+      </c>
+      <c r="H55" s="0">
+        <v>3</v>
+      </c>
+      <c r="I55" s="0" t="inlineStr"/>
+      <c r="J55" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K55" s="0" t="inlineStr">
+        <is>
+          <t>Coho</t>
+        </is>
+      </c>
+      <c r="L55" s="0">
+        <v>626</v>
+      </c>
+      <c r="M55" s="0">
+        <v>1</v>
+      </c>
+      <c r="N55" s="0">
+        <v>627</v>
+      </c>
+      <c r="O55" s="0">
+        <v>100</v>
+      </c>
+      <c r="Q55" s="0">
+        <v>100</v>
+      </c>
+      <c r="V55" s="0">
+        <v>0</v>
+      </c>
+      <c r="W55" s="0">
+        <v>1</v>
+      </c>
+      <c r="AB55" s="1">
+        <v>45624.412349537</v>
+      </c>
+      <c r="AC55" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="56">
+      <c r="A56" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B56" s="0" t="inlineStr">
+        <is>
+          <t>NITINAT RIVER</t>
+        </is>
+      </c>
+      <c r="C56" s="1">
+        <v>45609</v>
+      </c>
+      <c r="D56" s="0" t="inlineStr">
+        <is>
+          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E56" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F56" s="0" t="inlineStr">
+        <is>
+          <t>PK</t>
+        </is>
+      </c>
+      <c r="G56" s="0">
+        <v>8</v>
+      </c>
+      <c r="H56" s="0">
+        <v>3</v>
+      </c>
+      <c r="I56" s="0" t="inlineStr"/>
+      <c r="J56" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K56" s="0" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="N56" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="0">
+        <v>0</v>
+      </c>
+      <c r="V56" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB56" s="1">
+        <v>45624.412349537</v>
+      </c>
+      <c r="AC56" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="57">
+      <c r="A57" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B57" s="0" t="inlineStr">
+        <is>
+          <t>NITINAT RIVER</t>
+        </is>
+      </c>
+      <c r="C57" s="1">
+        <v>45609</v>
+      </c>
+      <c r="D57" s="0" t="inlineStr">
+        <is>
+          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E57" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F57" s="0" t="inlineStr">
+        <is>
+          <t>SK</t>
+        </is>
+      </c>
+      <c r="G57" s="0">
+        <v>8</v>
+      </c>
+      <c r="H57" s="0">
+        <v>3</v>
+      </c>
+      <c r="I57" s="0" t="inlineStr"/>
+      <c r="J57" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K57" s="0" t="inlineStr">
+        <is>
+          <t>Sockeye</t>
+        </is>
+      </c>
+      <c r="N57" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="0">
+        <v>0</v>
+      </c>
+      <c r="V57" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB57" s="1">
+        <v>45624.412349537</v>
+      </c>
+      <c r="AC57" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="58">
+      <c r="A58" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B58" s="0" t="inlineStr">
+        <is>
+          <t>WORTHLESS CREEK</t>
+        </is>
+      </c>
+      <c r="C58" s="1">
+        <v>45589</v>
+      </c>
+      <c r="D58" s="0" t="inlineStr">
+        <is>
+          <t>930-071700-44200-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E58" s="0" t="inlineStr">
+        <is>
+          <t>heli</t>
+        </is>
+      </c>
+      <c r="F58" s="0" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="G58" s="0">
+        <v>99</v>
+      </c>
+      <c r="H58" s="0">
+        <v>6</v>
+      </c>
+      <c r="I58" s="0" t="inlineStr">
+        <is>
+          <t>1 - 3 m</t>
+        </is>
+      </c>
+      <c r="J58" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K58" s="0" t="inlineStr">
+        <is>
+          <t>Chum</t>
+        </is>
+      </c>
+      <c r="L58" s="0">
+        <v>430</v>
+      </c>
+      <c r="N58" s="0">
+        <v>430</v>
+      </c>
+      <c r="Q58" s="0">
+        <v>0</v>
+      </c>
+      <c r="T58" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U58" s="0">
+        <v>0.899999976158142</v>
+      </c>
+      <c r="V58" s="0">
+        <v>0</v>
+      </c>
+      <c r="W58" s="0">
+        <v>1</v>
+      </c>
+      <c r="X58" s="0">
+        <v>478</v>
+      </c>
+      <c r="AB58" s="1">
+        <v>45624.412349537</v>
+      </c>
+      <c r="AC58" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="59">
+      <c r="A59" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B59" s="0" t="inlineStr">
+        <is>
+          <t>WORTHLESS CREEK</t>
+        </is>
+      </c>
+      <c r="C59" s="1">
+        <v>45589</v>
+      </c>
+      <c r="D59" s="0" t="inlineStr">
+        <is>
+          <t>930-071700-44200-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E59" s="0" t="inlineStr">
+        <is>
+          <t>heli</t>
+        </is>
+      </c>
+      <c r="F59" s="0" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G59" s="0">
+        <v>99</v>
+      </c>
+      <c r="H59" s="0">
+        <v>6</v>
+      </c>
+      <c r="I59" s="0" t="inlineStr">
+        <is>
+          <t>1 - 3 m</t>
+        </is>
+      </c>
+      <c r="J59" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K59" s="0" t="inlineStr">
+        <is>
+          <t>Chinook</t>
+        </is>
+      </c>
+      <c r="N59" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="0">
+        <v>0</v>
+      </c>
+      <c r="V59" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB59" s="1">
+        <v>45624.412349537</v>
+      </c>
+      <c r="AC59" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="60">
+      <c r="A60" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B60" s="0" t="inlineStr">
+        <is>
+          <t>WORTHLESS CREEK</t>
+        </is>
+      </c>
+      <c r="C60" s="1">
+        <v>45589</v>
+      </c>
+      <c r="D60" s="0" t="inlineStr">
+        <is>
+          <t>930-071700-44200-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E60" s="0" t="inlineStr">
+        <is>
+          <t>heli</t>
+        </is>
+      </c>
+      <c r="F60" s="0" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="G60" s="0">
+        <v>99</v>
+      </c>
+      <c r="H60" s="0">
+        <v>6</v>
+      </c>
+      <c r="I60" s="0" t="inlineStr">
+        <is>
+          <t>1 - 3 m</t>
+        </is>
+      </c>
+      <c r="J60" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K60" s="0" t="inlineStr">
+        <is>
+          <t>Coho</t>
+        </is>
+      </c>
+      <c r="N60" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="0">
+        <v>0</v>
+      </c>
+      <c r="V60" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB60" s="1">
+        <v>45624.412349537</v>
+      </c>
+      <c r="AC60" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="61">
+      <c r="A61" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B61" s="0" t="inlineStr">
+        <is>
+          <t>WORTHLESS CREEK</t>
+        </is>
+      </c>
+      <c r="C61" s="1">
+        <v>45589</v>
+      </c>
+      <c r="D61" s="0" t="inlineStr">
+        <is>
+          <t>930-071700-44200-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E61" s="0" t="inlineStr">
+        <is>
+          <t>heli</t>
+        </is>
+      </c>
+      <c r="F61" s="0" t="inlineStr">
+        <is>
+          <t>PK</t>
+        </is>
+      </c>
+      <c r="G61" s="0">
+        <v>99</v>
+      </c>
+      <c r="H61" s="0">
+        <v>6</v>
+      </c>
+      <c r="I61" s="0" t="inlineStr">
+        <is>
+          <t>1 - 3 m</t>
+        </is>
+      </c>
+      <c r="J61" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K61" s="0" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="N61" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="0">
+        <v>0</v>
+      </c>
+      <c r="V61" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB61" s="1">
+        <v>45624.412349537</v>
+      </c>
+      <c r="AC61" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="62">
+      <c r="A62" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B62" s="0" t="inlineStr">
+        <is>
+          <t>WORTHLESS CREEK</t>
+        </is>
+      </c>
+      <c r="C62" s="1">
+        <v>45589</v>
+      </c>
+      <c r="D62" s="0" t="inlineStr">
+        <is>
+          <t>930-071700-44200-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E62" s="0" t="inlineStr">
+        <is>
+          <t>heli</t>
+        </is>
+      </c>
+      <c r="F62" s="0" t="inlineStr">
+        <is>
+          <t>SK</t>
+        </is>
+      </c>
+      <c r="G62" s="0">
+        <v>99</v>
+      </c>
+      <c r="H62" s="0">
+        <v>6</v>
+      </c>
+      <c r="I62" s="0" t="inlineStr">
+        <is>
+          <t>1 - 3 m</t>
+        </is>
+      </c>
+      <c r="J62" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K62" s="0" t="inlineStr">
+        <is>
+          <t>Sockeye</t>
+        </is>
+      </c>
+      <c r="N62" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="0">
+        <v>0</v>
+      </c>
+      <c r="V62" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB62" s="1">
+        <v>45624.412349537</v>
+      </c>
+      <c r="AC62" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="63">
+      <c r="A63" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B63" s="0" t="inlineStr">
+        <is>
+          <t>WORTHLESS CREEK</t>
+        </is>
+      </c>
+      <c r="C63" s="1">
+        <v>45597</v>
+      </c>
+      <c r="D63" s="0" t="inlineStr">
+        <is>
+          <t>930-071700-44200-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E63" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F63" s="0" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="G63" s="0">
+        <v>99</v>
+      </c>
+      <c r="H63" s="0">
+        <v>3</v>
+      </c>
+      <c r="I63" s="0" t="inlineStr">
+        <is>
           <t>3 - 5 m or to Bottom</t>
         </is>
       </c>
-      <c r="J52" s="0" t="inlineStr">
+      <c r="J63" s="0" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="K52" s="0" t="inlineStr">
+      <c r="K63" s="0" t="inlineStr">
+        <is>
+          <t>Chum</t>
+        </is>
+      </c>
+      <c r="L63" s="0">
+        <v>27</v>
+      </c>
+      <c r="M63" s="0">
+        <v>186</v>
+      </c>
+      <c r="N63" s="0">
+        <v>213</v>
+      </c>
+      <c r="Q63" s="0">
+        <v>0</v>
+      </c>
+      <c r="V63" s="0">
+        <v>0</v>
+      </c>
+      <c r="W63" s="0">
+        <v>0.899999976158142</v>
+      </c>
+      <c r="AB63" s="1">
+        <v>45624.412349537</v>
+      </c>
+      <c r="AC63" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="64">
+      <c r="A64" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B64" s="0" t="inlineStr">
+        <is>
+          <t>WORTHLESS CREEK</t>
+        </is>
+      </c>
+      <c r="C64" s="1">
+        <v>45597</v>
+      </c>
+      <c r="D64" s="0" t="inlineStr">
+        <is>
+          <t>930-071700-44200-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E64" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F64" s="0" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G64" s="0">
+        <v>99</v>
+      </c>
+      <c r="H64" s="0">
+        <v>3</v>
+      </c>
+      <c r="I64" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J64" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K64" s="0" t="inlineStr">
+        <is>
+          <t>Chinook</t>
+        </is>
+      </c>
+      <c r="N64" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="0">
+        <v>0</v>
+      </c>
+      <c r="V64" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB64" s="1">
+        <v>45624.412349537</v>
+      </c>
+      <c r="AC64" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="65">
+      <c r="A65" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B65" s="0" t="inlineStr">
+        <is>
+          <t>WORTHLESS CREEK</t>
+        </is>
+      </c>
+      <c r="C65" s="1">
+        <v>45597</v>
+      </c>
+      <c r="D65" s="0" t="inlineStr">
+        <is>
+          <t>930-071700-44200-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E65" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F65" s="0" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="G65" s="0">
+        <v>99</v>
+      </c>
+      <c r="H65" s="0">
+        <v>3</v>
+      </c>
+      <c r="I65" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J65" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K65" s="0" t="inlineStr">
+        <is>
+          <t>Coho</t>
+        </is>
+      </c>
+      <c r="L65" s="0">
+        <v>36</v>
+      </c>
+      <c r="M65" s="0">
+        <v>0</v>
+      </c>
+      <c r="N65" s="0">
+        <v>36</v>
+      </c>
+      <c r="O65" s="0">
+        <v>8</v>
+      </c>
+      <c r="Q65" s="0">
+        <v>8</v>
+      </c>
+      <c r="V65" s="0">
+        <v>0</v>
+      </c>
+      <c r="W65" s="0">
+        <v>0.899999976158142</v>
+      </c>
+      <c r="AB65" s="1">
+        <v>45624.412349537</v>
+      </c>
+      <c r="AC65" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="66">
+      <c r="A66" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B66" s="0" t="inlineStr">
+        <is>
+          <t>WORTHLESS CREEK</t>
+        </is>
+      </c>
+      <c r="C66" s="1">
+        <v>45597</v>
+      </c>
+      <c r="D66" s="0" t="inlineStr">
+        <is>
+          <t>930-071700-44200-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E66" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F66" s="0" t="inlineStr">
+        <is>
+          <t>PK</t>
+        </is>
+      </c>
+      <c r="G66" s="0">
+        <v>99</v>
+      </c>
+      <c r="H66" s="0">
+        <v>3</v>
+      </c>
+      <c r="I66" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J66" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K66" s="0" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="N66" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="0">
+        <v>0</v>
+      </c>
+      <c r="V66" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB66" s="1">
+        <v>45624.412349537</v>
+      </c>
+      <c r="AC66" s="0" t="inlineStr">
+        <is>
+          <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="67">
+      <c r="A67" s="0">
+        <v>2024</v>
+      </c>
+      <c r="B67" s="0" t="inlineStr">
+        <is>
+          <t>WORTHLESS CREEK</t>
+        </is>
+      </c>
+      <c r="C67" s="1">
+        <v>45597</v>
+      </c>
+      <c r="D67" s="0" t="inlineStr">
+        <is>
+          <t>930-071700-44200-00000-0000-0000-000-000-000-000-000-000</t>
+        </is>
+      </c>
+      <c r="E67" s="0" t="inlineStr">
+        <is>
+          <t>snrkl</t>
+        </is>
+      </c>
+      <c r="F67" s="0" t="inlineStr">
+        <is>
+          <t>SK</t>
+        </is>
+      </c>
+      <c r="G67" s="0">
+        <v>99</v>
+      </c>
+      <c r="H67" s="0">
+        <v>3</v>
+      </c>
+      <c r="I67" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
+      <c r="J67" s="0" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="K67" s="0" t="inlineStr">
         <is>
           <t>Sockeye</t>
         </is>
       </c>
-      <c r="N52" s="0">
-        <v>0</v>
-      </c>
-      <c r="Q52" s="0">
-        <v>0</v>
-      </c>
-      <c r="V52" s="0">
-        <v>0</v>
-      </c>
-      <c r="AB52" s="1">
-        <v>45624.3850810185</v>
-      </c>
-      <c r="AC52" s="0" t="inlineStr">
+      <c r="N67" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="0">
+        <v>0</v>
+      </c>
+      <c r="V67" s="0">
+        <v>0</v>
+      </c>
+      <c r="AB67" s="1">
+        <v>45624.412349537</v>
+      </c>
+      <c r="AC67" s="0" t="inlineStr">
         <is>
           <t>Z:\WCVI\ESCAPEMENT\Data\2024\2024 SIL+AUC database\SIL+AUC Database v9.1_2024_A20-21-22_WCVI.accdb</t>
         </is>

</xml_diff>

<commit_message>
updated SIL+AUC database outputs
</commit_message>
<xml_diff>
--- a/data/escapement/prelim-inseason/AUC_DataAnalysisTable_area21-22_2024.xlsx
+++ b/data/escapement/prelim-inseason/AUC_DataAnalysisTable_area21-22_2024.xlsx
@@ -568,7 +568,7 @@
         </is>
       </c>
       <c r="U2" s="0">
-        <v>0.949999988079071</v>
+        <v>0.800000011920929</v>
       </c>
       <c r="V2" s="0">
         <v>0</v>
@@ -577,10 +577,10 @@
         <v>0.801214814186096</v>
       </c>
       <c r="X2" s="0">
-        <v>1906</v>
+        <v>2264</v>
       </c>
       <c r="AB2" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC2" s="0" t="inlineStr">
         <is>
@@ -651,7 +651,7 @@
         </is>
       </c>
       <c r="U3" s="0">
-        <v>1</v>
+        <v>0.600000023841858</v>
       </c>
       <c r="V3" s="0">
         <v>0</v>
@@ -660,10 +660,10 @@
         <v>0.5</v>
       </c>
       <c r="X3" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB3" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC3" s="0" t="inlineStr">
         <is>
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="U4" s="0">
-        <v>1</v>
+        <v>0.899999976158142</v>
       </c>
       <c r="V4" s="0">
         <v>0</v>
@@ -749,10 +749,10 @@
         <v>0.800000011920929</v>
       </c>
       <c r="X4" s="0">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="AB4" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC4" s="0" t="inlineStr">
         <is>
@@ -823,7 +823,7 @@
         <v>0</v>
       </c>
       <c r="AB5" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC5" s="0" t="inlineStr">
         <is>
@@ -889,7 +889,7 @@
         <v>0</v>
       </c>
       <c r="AB6" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC6" s="0" t="inlineStr">
         <is>
@@ -903,20 +903,20 @@
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>LITTLE NITINAT RIVER</t>
+          <t>CAMPUS CREEK</t>
         </is>
       </c>
       <c r="C7" s="1">
-        <v>45589</v>
+        <v>45598</v>
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>930-071700-37600-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-28000-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E7" s="0" t="inlineStr">
         <is>
-          <t>heli</t>
+          <t>snrkl</t>
         </is>
       </c>
       <c r="F7" s="0" t="inlineStr">
@@ -925,14 +925,14 @@
         </is>
       </c>
       <c r="G7" s="0">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="H7" s="0">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I7" s="0" t="inlineStr">
         <is>
-          <t>1 - 3 m</t>
+          <t>3 - 5 m or to Bottom</t>
         </is>
       </c>
       <c r="J7" s="0" t="inlineStr">
@@ -946,33 +946,25 @@
         </is>
       </c>
       <c r="L7" s="0">
-        <v>380</v>
+        <v>187</v>
+      </c>
+      <c r="M7" s="0">
+        <v>851</v>
       </c>
       <c r="N7" s="0">
-        <v>380</v>
+        <v>1038</v>
       </c>
       <c r="Q7" s="0">
         <v>0</v>
       </c>
-      <c r="T7" s="0" t="inlineStr">
-        <is>
-          <t>H</t>
-        </is>
-      </c>
-      <c r="U7" s="0">
-        <v>1</v>
-      </c>
       <c r="V7" s="0">
         <v>0</v>
       </c>
       <c r="W7" s="0">
-        <v>1</v>
-      </c>
-      <c r="X7" s="0">
-        <v>380</v>
+        <v>0.94923859834671</v>
       </c>
       <c r="AB7" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC7" s="0" t="inlineStr">
         <is>
@@ -986,20 +978,20 @@
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>LITTLE NITINAT RIVER</t>
+          <t>CAMPUS CREEK</t>
         </is>
       </c>
       <c r="C8" s="1">
-        <v>45589</v>
+        <v>45598</v>
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>930-071700-37600-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-28000-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E8" s="0" t="inlineStr">
         <is>
-          <t>heli</t>
+          <t>snrkl</t>
         </is>
       </c>
       <c r="F8" s="0" t="inlineStr">
@@ -1008,14 +1000,14 @@
         </is>
       </c>
       <c r="G8" s="0">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="H8" s="0">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I8" s="0" t="inlineStr">
         <is>
-          <t>1 - 3 m</t>
+          <t>3 - 5 m or to Bottom</t>
         </is>
       </c>
       <c r="J8" s="0" t="inlineStr">
@@ -1038,7 +1030,7 @@
         <v>0</v>
       </c>
       <c r="AB8" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC8" s="0" t="inlineStr">
         <is>
@@ -1052,20 +1044,20 @@
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>LITTLE NITINAT RIVER</t>
+          <t>CAMPUS CREEK</t>
         </is>
       </c>
       <c r="C9" s="1">
-        <v>45589</v>
+        <v>45598</v>
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>930-071700-37600-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-28000-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E9" s="0" t="inlineStr">
         <is>
-          <t>heli</t>
+          <t>snrkl</t>
         </is>
       </c>
       <c r="F9" s="0" t="inlineStr">
@@ -1074,14 +1066,14 @@
         </is>
       </c>
       <c r="G9" s="0">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="H9" s="0">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I9" s="0" t="inlineStr">
         <is>
-          <t>1 - 3 m</t>
+          <t>3 - 5 m or to Bottom</t>
         </is>
       </c>
       <c r="J9" s="0" t="inlineStr">
@@ -1094,17 +1086,29 @@
           <t>Coho</t>
         </is>
       </c>
+      <c r="L9" s="0">
+        <v>12</v>
+      </c>
+      <c r="M9" s="0">
+        <v>1</v>
+      </c>
       <c r="N9" s="0">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="O9" s="0">
+        <v>1</v>
       </c>
       <c r="Q9" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9" s="0">
         <v>0</v>
       </c>
+      <c r="W9" s="0">
+        <v>0.923076927661896</v>
+      </c>
       <c r="AB9" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC9" s="0" t="inlineStr">
         <is>
@@ -1118,20 +1122,20 @@
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>LITTLE NITINAT RIVER</t>
+          <t>CAMPUS CREEK</t>
         </is>
       </c>
       <c r="C10" s="1">
-        <v>45589</v>
+        <v>45598</v>
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>930-071700-37600-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-28000-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E10" s="0" t="inlineStr">
         <is>
-          <t>heli</t>
+          <t>snrkl</t>
         </is>
       </c>
       <c r="F10" s="0" t="inlineStr">
@@ -1140,14 +1144,14 @@
         </is>
       </c>
       <c r="G10" s="0">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="H10" s="0">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I10" s="0" t="inlineStr">
         <is>
-          <t>1 - 3 m</t>
+          <t>3 - 5 m or to Bottom</t>
         </is>
       </c>
       <c r="J10" s="0" t="inlineStr">
@@ -1160,22 +1164,17 @@
           <t>Pink</t>
         </is>
       </c>
-      <c r="L10" s="0"/>
       <c r="N10" s="0">
         <v>0</v>
       </c>
       <c r="Q10" s="0">
         <v>0</v>
       </c>
-      <c r="T10" s="0" t="inlineStr"/>
-      <c r="U10" s="0"/>
       <c r="V10" s="0">
         <v>0</v>
       </c>
-      <c r="W10" s="0"/>
-      <c r="X10" s="0"/>
       <c r="AB10" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC10" s="0" t="inlineStr">
         <is>
@@ -1189,20 +1188,20 @@
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>LITTLE NITINAT RIVER</t>
+          <t>CAMPUS CREEK</t>
         </is>
       </c>
       <c r="C11" s="1">
-        <v>45589</v>
+        <v>45598</v>
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>930-071700-37600-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-28000-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E11" s="0" t="inlineStr">
         <is>
-          <t>heli</t>
+          <t>snrkl</t>
         </is>
       </c>
       <c r="F11" s="0" t="inlineStr">
@@ -1211,14 +1210,14 @@
         </is>
       </c>
       <c r="G11" s="0">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="H11" s="0">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I11" s="0" t="inlineStr">
         <is>
-          <t>1 - 3 m</t>
+          <t>3 - 5 m or to Bottom</t>
         </is>
       </c>
       <c r="J11" s="0" t="inlineStr">
@@ -1241,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="AB11" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC11" s="0" t="inlineStr">
         <is>
@@ -1255,20 +1254,20 @@
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>NITINAT RIVER</t>
+          <t>LITTLE NITINAT RIVER</t>
         </is>
       </c>
       <c r="C12" s="1">
-        <v>45504</v>
+        <v>45589</v>
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-37600-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E12" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F12" s="0" t="inlineStr">
@@ -1277,19 +1276,19 @@
         </is>
       </c>
       <c r="G12" s="0">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="H12" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I12" s="0" t="inlineStr">
         <is>
-          <t>3 - 5 m or to Bottom</t>
+          <t>1 - 3 m</t>
         </is>
       </c>
       <c r="J12" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K12" s="0" t="inlineStr">
@@ -1298,17 +1297,17 @@
         </is>
       </c>
       <c r="L12" s="0">
-        <v>1</v>
+        <v>380</v>
       </c>
       <c r="N12" s="0">
-        <v>1</v>
+        <v>380</v>
       </c>
       <c r="Q12" s="0">
         <v>0</v>
       </c>
       <c r="T12" s="0" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
       <c r="U12" s="0">
@@ -1321,10 +1320,10 @@
         <v>1</v>
       </c>
       <c r="X12" s="0">
-        <v>1</v>
+        <v>380</v>
       </c>
       <c r="AB12" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC12" s="0" t="inlineStr">
         <is>
@@ -1338,20 +1337,20 @@
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>NITINAT RIVER</t>
+          <t>LITTLE NITINAT RIVER</t>
         </is>
       </c>
       <c r="C13" s="1">
-        <v>45504</v>
+        <v>45589</v>
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-37600-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E13" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F13" s="0" t="inlineStr">
@@ -1360,19 +1359,19 @@
         </is>
       </c>
       <c r="G13" s="0">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="H13" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I13" s="0" t="inlineStr">
         <is>
-          <t>3 - 5 m or to Bottom</t>
+          <t>1 - 3 m</t>
         </is>
       </c>
       <c r="J13" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K13" s="0" t="inlineStr">
@@ -1380,7 +1379,6 @@
           <t>Chinook</t>
         </is>
       </c>
-      <c r="L13" s="0"/>
       <c r="N13" s="0">
         <v>0</v>
       </c>
@@ -1391,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="AB13" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC13" s="0" t="inlineStr">
         <is>
@@ -1405,20 +1403,20 @@
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>NITINAT RIVER</t>
+          <t>LITTLE NITINAT RIVER</t>
         </is>
       </c>
       <c r="C14" s="1">
-        <v>45504</v>
+        <v>45589</v>
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-37600-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E14" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F14" s="0" t="inlineStr">
@@ -1427,19 +1425,19 @@
         </is>
       </c>
       <c r="G14" s="0">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="H14" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I14" s="0" t="inlineStr">
         <is>
-          <t>3 - 5 m or to Bottom</t>
+          <t>1 - 3 m</t>
         </is>
       </c>
       <c r="J14" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K14" s="0" t="inlineStr">
@@ -1447,24 +1445,17 @@
           <t>Coho</t>
         </is>
       </c>
-      <c r="L14" s="0"/>
-      <c r="M14" s="0"/>
       <c r="N14" s="0">
         <v>0</v>
       </c>
-      <c r="O14" s="0"/>
       <c r="Q14" s="0">
         <v>0</v>
       </c>
-      <c r="T14" s="0" t="inlineStr"/>
-      <c r="U14" s="0"/>
       <c r="V14" s="0">
         <v>0</v>
       </c>
-      <c r="W14" s="0"/>
-      <c r="X14" s="0"/>
       <c r="AB14" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC14" s="0" t="inlineStr">
         <is>
@@ -1478,78 +1469,59 @@
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>NITINAT RIVER</t>
+          <t>LITTLE NITINAT RIVER</t>
         </is>
       </c>
       <c r="C15" s="1">
-        <v>45504</v>
+        <v>45589</v>
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-37600-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E15" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F15" s="0" t="inlineStr">
         <is>
-          <t>OT</t>
+          <t>PK</t>
         </is>
       </c>
       <c r="G15" s="0">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="H15" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I15" s="0" t="inlineStr">
         <is>
-          <t>3 - 5 m or to Bottom</t>
+          <t>1 - 3 m</t>
         </is>
       </c>
       <c r="J15" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K15" s="0" t="inlineStr">
         <is>
-          <t>Cutthroat</t>
-        </is>
-      </c>
-      <c r="L15" s="0">
-        <v>32</v>
-      </c>
-      <c r="M15" s="0"/>
+          <t>Pink</t>
+        </is>
+      </c>
       <c r="N15" s="0">
-        <v>32</v>
-      </c>
-      <c r="O15" s="0"/>
+        <v>0</v>
+      </c>
       <c r="Q15" s="0">
         <v>0</v>
       </c>
-      <c r="T15" s="0" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="U15" s="0">
-        <v>0.850000023841858</v>
-      </c>
       <c r="V15" s="0">
         <v>0</v>
       </c>
-      <c r="W15" s="0">
-        <v>0.864864885807037</v>
-      </c>
-      <c r="X15" s="0">
-        <v>44</v>
-      </c>
       <c r="AB15" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC15" s="0" t="inlineStr">
         <is>
@@ -1563,49 +1535,48 @@
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>NITINAT RIVER</t>
+          <t>LITTLE NITINAT RIVER</t>
         </is>
       </c>
       <c r="C16" s="1">
-        <v>45504</v>
+        <v>45589</v>
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>930-071700-00000-00000-0000-0000-000-000-000-000-000-000</t>
+          <t>930-071700-37600-00000-0000-0000-000-000-000-000-000-000</t>
         </is>
       </c>
       <c r="E16" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F16" s="0" t="inlineStr">
         <is>
-          <t>PK</t>
+          <t>SK</t>
         </is>
       </c>
       <c r="G16" s="0">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="H16" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I16" s="0" t="inlineStr">
         <is>
-          <t>3 - 5 m or to Bottom</t>
+          <t>1 - 3 m</t>
         </is>
       </c>
       <c r="J16" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K16" s="0" t="inlineStr">
         <is>
-          <t>Pink</t>
-        </is>
-      </c>
-      <c r="L16" s="0"/>
+          <t>Sockeye</t>
+        </is>
+      </c>
       <c r="N16" s="0">
         <v>0</v>
       </c>
@@ -1616,7 +1587,7 @@
         <v>0</v>
       </c>
       <c r="AB16" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC16" s="0" t="inlineStr">
         <is>
@@ -1648,7 +1619,7 @@
       </c>
       <c r="F17" s="0" t="inlineStr">
         <is>
-          <t>SK</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="G17" s="0">
@@ -1669,15 +1640,14 @@
       </c>
       <c r="K17" s="0" t="inlineStr">
         <is>
-          <t>Sockeye</t>
+          <t>Chum</t>
         </is>
       </c>
       <c r="L17" s="0">
-        <v>65</v>
-      </c>
-      <c r="M17" s="0"/>
+        <v>1</v>
+      </c>
       <c r="N17" s="0">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="0">
         <v>0</v>
@@ -1688,19 +1658,19 @@
         </is>
       </c>
       <c r="U17" s="0">
-        <v>0.850000023841858</v>
+        <v>1</v>
       </c>
       <c r="V17" s="0">
         <v>0</v>
       </c>
       <c r="W17" s="0">
-        <v>0.866666674613953</v>
+        <v>1</v>
       </c>
       <c r="X17" s="0">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="AB17" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC17" s="0" t="inlineStr">
         <is>
@@ -1718,7 +1688,7 @@
         </is>
       </c>
       <c r="C18" s="1">
-        <v>45539</v>
+        <v>45504</v>
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
@@ -1732,11 +1702,11 @@
       </c>
       <c r="F18" s="0" t="inlineStr">
         <is>
-          <t>CM</t>
+          <t>CN</t>
         </is>
       </c>
       <c r="G18" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H18" s="0">
         <v>3</v>
@@ -1748,33 +1718,25 @@
       </c>
       <c r="J18" s="0" t="inlineStr">
         <is>
-          <t>Extremely Low</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K18" s="0" t="inlineStr">
         <is>
-          <t>Chum</t>
-        </is>
-      </c>
-      <c r="L18" s="0">
-        <v>0</v>
-      </c>
-      <c r="M18" s="0"/>
+          <t>Chinook</t>
+        </is>
+      </c>
       <c r="N18" s="0">
         <v>0</v>
       </c>
       <c r="Q18" s="0">
         <v>0</v>
       </c>
-      <c r="T18" s="0" t="inlineStr"/>
-      <c r="U18" s="0"/>
       <c r="V18" s="0">
         <v>0</v>
       </c>
-      <c r="W18" s="0"/>
-      <c r="X18" s="0"/>
       <c r="AB18" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC18" s="0" t="inlineStr">
         <is>
@@ -1792,7 +1754,7 @@
         </is>
       </c>
       <c r="C19" s="1">
-        <v>45539</v>
+        <v>45504</v>
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
@@ -1806,11 +1768,11 @@
       </c>
       <c r="F19" s="0" t="inlineStr">
         <is>
-          <t>CN</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="G19" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H19" s="0">
         <v>3</v>
@@ -1822,48 +1784,25 @@
       </c>
       <c r="J19" s="0" t="inlineStr">
         <is>
-          <t>Extremely Low</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K19" s="0" t="inlineStr">
         <is>
-          <t>Chinook</t>
-        </is>
-      </c>
-      <c r="L19" s="0">
-        <v>1955</v>
-      </c>
-      <c r="M19" s="0">
-        <v>0</v>
+          <t>Coho</t>
+        </is>
       </c>
       <c r="N19" s="0">
-        <v>1955</v>
-      </c>
-      <c r="O19" s="0">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="Q19" s="0">
-        <v>23</v>
-      </c>
-      <c r="T19" s="0" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="U19" s="0">
-        <v>0.850000023841858</v>
+        <v>0</v>
       </c>
       <c r="V19" s="0">
         <v>0</v>
       </c>
-      <c r="W19" s="0">
-        <v>0.882618486881256</v>
-      </c>
-      <c r="X19" s="0">
-        <v>2606</v>
-      </c>
       <c r="AB19" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC19" s="0" t="inlineStr">
         <is>
@@ -1881,7 +1820,7 @@
         </is>
       </c>
       <c r="C20" s="1">
-        <v>45539</v>
+        <v>45504</v>
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
@@ -1895,11 +1834,11 @@
       </c>
       <c r="F20" s="0" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>OT</t>
         </is>
       </c>
       <c r="G20" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H20" s="0">
         <v>3</v>
@@ -1911,48 +1850,42 @@
       </c>
       <c r="J20" s="0" t="inlineStr">
         <is>
-          <t>Extremely Low</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K20" s="0" t="inlineStr">
         <is>
-          <t>Coho</t>
+          <t>Cutthroat</t>
         </is>
       </c>
       <c r="L20" s="0">
-        <v>120</v>
-      </c>
-      <c r="M20" s="0">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N20" s="0">
-        <v>120</v>
-      </c>
-      <c r="O20" s="0">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="Q20" s="0">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="T20" s="0" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
       <c r="U20" s="0">
-        <v>1</v>
+        <v>0.850000023841858</v>
       </c>
       <c r="V20" s="0">
         <v>0</v>
       </c>
       <c r="W20" s="0">
-        <v>0.967741906642914</v>
+        <v>0.864864885807037</v>
       </c>
       <c r="X20" s="0">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="AB20" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC20" s="0" t="inlineStr">
         <is>
@@ -1970,7 +1903,7 @@
         </is>
       </c>
       <c r="C21" s="1">
-        <v>45539</v>
+        <v>45504</v>
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
@@ -1988,7 +1921,7 @@
         </is>
       </c>
       <c r="G21" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H21" s="0">
         <v>3</v>
@@ -2000,7 +1933,7 @@
       </c>
       <c r="J21" s="0" t="inlineStr">
         <is>
-          <t>Extremely Low</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K21" s="0" t="inlineStr">
@@ -2008,22 +1941,17 @@
           <t>Pink</t>
         </is>
       </c>
-      <c r="L21" s="0">
-        <v>0</v>
-      </c>
       <c r="N21" s="0">
         <v>0</v>
       </c>
       <c r="Q21" s="0">
         <v>0</v>
       </c>
-      <c r="T21" s="0" t="inlineStr"/>
-      <c r="U21" s="0"/>
       <c r="V21" s="0">
         <v>0</v>
       </c>
       <c r="AB21" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC21" s="0" t="inlineStr">
         <is>
@@ -2041,7 +1969,7 @@
         </is>
       </c>
       <c r="C22" s="1">
-        <v>45539</v>
+        <v>45504</v>
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
@@ -2059,7 +1987,7 @@
         </is>
       </c>
       <c r="G22" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H22" s="0">
         <v>3</v>
@@ -2071,7 +1999,7 @@
       </c>
       <c r="J22" s="0" t="inlineStr">
         <is>
-          <t>Extremely Low</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K22" s="0" t="inlineStr">
@@ -2080,37 +2008,33 @@
         </is>
       </c>
       <c r="L22" s="0">
-        <v>230</v>
-      </c>
-      <c r="M22" s="0">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="N22" s="0">
-        <v>230</v>
-      </c>
-      <c r="O22" s="0"/>
+        <v>65</v>
+      </c>
       <c r="Q22" s="0">
         <v>0</v>
       </c>
       <c r="T22" s="0" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
       <c r="U22" s="0">
-        <v>1</v>
+        <v>0.850000023841858</v>
       </c>
       <c r="V22" s="0">
         <v>0</v>
       </c>
       <c r="W22" s="0">
-        <v>0.962343096733093</v>
+        <v>0.866666674613953</v>
       </c>
       <c r="X22" s="0">
-        <v>239</v>
+        <v>88</v>
       </c>
       <c r="AB22" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC22" s="0" t="inlineStr">
         <is>
@@ -2128,7 +2052,7 @@
         </is>
       </c>
       <c r="C23" s="1">
-        <v>45555</v>
+        <v>45539</v>
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
@@ -2146,7 +2070,7 @@
         </is>
       </c>
       <c r="G23" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H23" s="0">
         <v>3</v>
@@ -2167,36 +2091,19 @@
         </is>
       </c>
       <c r="L23" s="0">
-        <v>81</v>
-      </c>
-      <c r="M23" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N23" s="0">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="0">
         <v>0</v>
       </c>
-      <c r="T23" s="0" t="inlineStr">
-        <is>
-          <t>H</t>
-        </is>
-      </c>
-      <c r="U23" s="0">
-        <v>1</v>
-      </c>
       <c r="V23" s="0">
         <v>0</v>
       </c>
-      <c r="W23" s="0">
-        <v>0.920454561710358</v>
-      </c>
-      <c r="X23" s="0">
-        <v>88</v>
-      </c>
       <c r="AB23" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC23" s="0" t="inlineStr">
         <is>
@@ -2214,7 +2121,7 @@
         </is>
       </c>
       <c r="C24" s="1">
-        <v>45555</v>
+        <v>45539</v>
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
@@ -2232,7 +2139,7 @@
         </is>
       </c>
       <c r="G24" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H24" s="0">
         <v>3</v>
@@ -2253,19 +2160,19 @@
         </is>
       </c>
       <c r="L24" s="0">
-        <v>7293</v>
+        <v>1955</v>
       </c>
       <c r="M24" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N24" s="0">
-        <v>7296</v>
+        <v>1955</v>
       </c>
       <c r="O24" s="0">
-        <v>295</v>
+        <v>23</v>
       </c>
       <c r="Q24" s="0">
-        <v>295</v>
+        <v>23</v>
       </c>
       <c r="T24" s="0" t="inlineStr">
         <is>
@@ -2273,19 +2180,19 @@
         </is>
       </c>
       <c r="U24" s="0">
-        <v>1</v>
+        <v>0.899999976158142</v>
       </c>
       <c r="V24" s="0">
         <v>0</v>
       </c>
       <c r="W24" s="0">
-        <v>0.90293425321579</v>
+        <v>0.882618486881256</v>
       </c>
       <c r="X24" s="0">
-        <v>8077</v>
+        <v>2461</v>
       </c>
       <c r="AB24" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC24" s="0" t="inlineStr">
         <is>
@@ -2303,7 +2210,7 @@
         </is>
       </c>
       <c r="C25" s="1">
-        <v>45555</v>
+        <v>45539</v>
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
@@ -2321,7 +2228,7 @@
         </is>
       </c>
       <c r="G25" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H25" s="0">
         <v>3</v>
@@ -2342,19 +2249,19 @@
         </is>
       </c>
       <c r="L25" s="0">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="M25" s="0">
         <v>0</v>
       </c>
       <c r="N25" s="0">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="O25" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q25" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T25" s="0" t="inlineStr">
         <is>
@@ -2368,13 +2275,13 @@
         <v>0</v>
       </c>
       <c r="W25" s="0">
-        <v>1</v>
+        <v>0.967741906642914</v>
       </c>
       <c r="X25" s="0">
-        <v>7</v>
+        <v>124</v>
       </c>
       <c r="AB25" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC25" s="0" t="inlineStr">
         <is>
@@ -2392,7 +2299,7 @@
         </is>
       </c>
       <c r="C26" s="1">
-        <v>45555</v>
+        <v>45539</v>
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
@@ -2410,7 +2317,7 @@
         </is>
       </c>
       <c r="G26" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H26" s="0">
         <v>3</v>
@@ -2430,26 +2337,20 @@
           <t>Pink</t>
         </is>
       </c>
-      <c r="L26" s="0"/>
+      <c r="L26" s="0">
+        <v>0</v>
+      </c>
       <c r="N26" s="0">
         <v>0</v>
       </c>
       <c r="Q26" s="0">
         <v>0</v>
       </c>
-      <c r="T26" s="0" t="inlineStr">
-        <is>
-          <t>H</t>
-        </is>
-      </c>
-      <c r="U26" s="0">
-        <v>1</v>
-      </c>
       <c r="V26" s="0">
         <v>0</v>
       </c>
       <c r="AB26" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC26" s="0" t="inlineStr">
         <is>
@@ -2467,7 +2368,7 @@
         </is>
       </c>
       <c r="C27" s="1">
-        <v>45555</v>
+        <v>45539</v>
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
@@ -2485,7 +2386,7 @@
         </is>
       </c>
       <c r="G27" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H27" s="0">
         <v>3</v>
@@ -2506,16 +2407,13 @@
         </is>
       </c>
       <c r="L27" s="0">
-        <v>155</v>
+        <v>230</v>
       </c>
       <c r="M27" s="0">
         <v>0</v>
       </c>
       <c r="N27" s="0">
-        <v>155</v>
-      </c>
-      <c r="O27" s="0">
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="Q27" s="0">
         <v>0</v>
@@ -2526,19 +2424,19 @@
         </is>
       </c>
       <c r="U27" s="0">
-        <v>1</v>
+        <v>0.850000023841858</v>
       </c>
       <c r="V27" s="0">
         <v>0</v>
       </c>
       <c r="W27" s="0">
-        <v>0.950920224189758</v>
+        <v>0.962343096733093</v>
       </c>
       <c r="X27" s="0">
-        <v>163</v>
+        <v>281</v>
       </c>
       <c r="AB27" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC27" s="0" t="inlineStr">
         <is>
@@ -2556,7 +2454,7 @@
         </is>
       </c>
       <c r="C28" s="1">
-        <v>45566</v>
+        <v>45555</v>
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
@@ -2574,7 +2472,7 @@
         </is>
       </c>
       <c r="G28" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H28" s="0">
         <v>3</v>
@@ -2586,7 +2484,7 @@
       </c>
       <c r="J28" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Extremely Low</t>
         </is>
       </c>
       <c r="K28" s="0" t="inlineStr">
@@ -2595,36 +2493,36 @@
         </is>
       </c>
       <c r="L28" s="0">
-        <v>13858</v>
+        <v>81</v>
       </c>
       <c r="M28" s="0">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N28" s="0">
-        <v>13863</v>
+        <v>82</v>
       </c>
       <c r="Q28" s="0">
         <v>0</v>
       </c>
       <c r="T28" s="0" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
       <c r="U28" s="0">
-        <v>1</v>
+        <v>0.949999988079071</v>
       </c>
       <c r="V28" s="0">
         <v>0</v>
       </c>
       <c r="W28" s="0">
-        <v>0.845360815525055</v>
+        <v>0.920454561710358</v>
       </c>
       <c r="X28" s="0">
-        <v>16393</v>
+        <v>93</v>
       </c>
       <c r="AB28" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC28" s="0" t="inlineStr">
         <is>
@@ -2642,7 +2540,7 @@
         </is>
       </c>
       <c r="C29" s="1">
-        <v>45566</v>
+        <v>45555</v>
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
@@ -2660,7 +2558,7 @@
         </is>
       </c>
       <c r="G29" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H29" s="0">
         <v>3</v>
@@ -2672,7 +2570,7 @@
       </c>
       <c r="J29" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Extremely Low</t>
         </is>
       </c>
       <c r="K29" s="0" t="inlineStr">
@@ -2681,17 +2579,19 @@
         </is>
       </c>
       <c r="L29" s="0">
-        <v>6151</v>
+        <v>7293</v>
       </c>
       <c r="M29" s="0">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="N29" s="0">
-        <v>6173</v>
-      </c>
-      <c r="O29" s="0"/>
+        <v>7296</v>
+      </c>
+      <c r="O29" s="0">
+        <v>295</v>
+      </c>
       <c r="Q29" s="0">
-        <v>0</v>
+        <v>295</v>
       </c>
       <c r="T29" s="0" t="inlineStr">
         <is>
@@ -2699,19 +2599,19 @@
         </is>
       </c>
       <c r="U29" s="0">
-        <v>1</v>
+        <v>0.899999976158142</v>
       </c>
       <c r="V29" s="0">
         <v>0</v>
       </c>
       <c r="W29" s="0">
-        <v>0.84064507484436</v>
+        <v>0.90293425321579</v>
       </c>
       <c r="X29" s="0">
-        <v>7317</v>
+        <v>8974</v>
       </c>
       <c r="AB29" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC29" s="0" t="inlineStr">
         <is>
@@ -2729,7 +2629,7 @@
         </is>
       </c>
       <c r="C30" s="1">
-        <v>45566</v>
+        <v>45555</v>
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
@@ -2747,7 +2647,7 @@
         </is>
       </c>
       <c r="G30" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H30" s="0">
         <v>3</v>
@@ -2759,7 +2659,7 @@
       </c>
       <c r="J30" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Extremely Low</t>
         </is>
       </c>
       <c r="K30" s="0" t="inlineStr">
@@ -2768,20 +2668,23 @@
         </is>
       </c>
       <c r="L30" s="0">
-        <v>195</v>
+        <v>7</v>
+      </c>
+      <c r="M30" s="0">
+        <v>0</v>
       </c>
       <c r="N30" s="0">
-        <v>195</v>
+        <v>7</v>
       </c>
       <c r="O30" s="0">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="0">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T30" s="0" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
       <c r="U30" s="0">
@@ -2791,13 +2694,13 @@
         <v>0</v>
       </c>
       <c r="W30" s="0">
-        <v>0.840517222881317</v>
+        <v>1</v>
       </c>
       <c r="X30" s="0">
-        <v>232</v>
+        <v>7</v>
       </c>
       <c r="AB30" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC30" s="0" t="inlineStr">
         <is>
@@ -2815,7 +2718,7 @@
         </is>
       </c>
       <c r="C31" s="1">
-        <v>45566</v>
+        <v>45555</v>
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
@@ -2833,7 +2736,7 @@
         </is>
       </c>
       <c r="G31" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H31" s="0">
         <v>3</v>
@@ -2845,7 +2748,7 @@
       </c>
       <c r="J31" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Extremely Low</t>
         </is>
       </c>
       <c r="K31" s="0" t="inlineStr">
@@ -2862,11 +2765,22 @@
       <c r="Q31" s="0">
         <v>0</v>
       </c>
+      <c r="T31" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U31" s="0">
+        <v>1</v>
+      </c>
       <c r="V31" s="0">
         <v>0</v>
       </c>
+      <c r="X31" s="0">
+        <v>0</v>
+      </c>
       <c r="AB31" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC31" s="0" t="inlineStr">
         <is>
@@ -2884,7 +2798,7 @@
         </is>
       </c>
       <c r="C32" s="1">
-        <v>45566</v>
+        <v>45555</v>
       </c>
       <c r="D32" s="0" t="inlineStr">
         <is>
@@ -2902,7 +2816,7 @@
         </is>
       </c>
       <c r="G32" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H32" s="0">
         <v>3</v>
@@ -2914,7 +2828,7 @@
       </c>
       <c r="J32" s="0" t="inlineStr">
         <is>
-          <t>Below Norm</t>
+          <t>Extremely Low</t>
         </is>
       </c>
       <c r="K32" s="0" t="inlineStr">
@@ -2923,34 +2837,39 @@
         </is>
       </c>
       <c r="L32" s="0">
-        <v>42</v>
+        <v>155</v>
+      </c>
+      <c r="M32" s="0">
+        <v>0</v>
       </c>
       <c r="N32" s="0">
-        <v>42</v>
-      </c>
-      <c r="O32" s="0"/>
+        <v>155</v>
+      </c>
+      <c r="O32" s="0">
+        <v>0</v>
+      </c>
       <c r="Q32" s="0">
         <v>0</v>
       </c>
       <c r="T32" s="0" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
       <c r="U32" s="0">
-        <v>1</v>
+        <v>0.850000023841858</v>
       </c>
       <c r="V32" s="0">
         <v>0</v>
       </c>
       <c r="W32" s="0">
-        <v>0.531645596027374</v>
+        <v>0.950920224189758</v>
       </c>
       <c r="X32" s="0">
-        <v>79</v>
+        <v>192</v>
       </c>
       <c r="AB32" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC32" s="0" t="inlineStr">
         <is>
@@ -2968,7 +2887,7 @@
         </is>
       </c>
       <c r="C33" s="1">
-        <v>45576</v>
+        <v>45566</v>
       </c>
       <c r="D33" s="0" t="inlineStr">
         <is>
@@ -2991,7 +2910,11 @@
       <c r="H33" s="0">
         <v>3</v>
       </c>
-      <c r="I33" s="0" t="inlineStr"/>
+      <c r="I33" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
       <c r="J33" s="0" t="inlineStr">
         <is>
           <t>Below Norm</t>
@@ -3003,20 +2926,20 @@
         </is>
       </c>
       <c r="L33" s="0">
-        <v>51744</v>
+        <v>13858</v>
       </c>
       <c r="M33" s="0">
-        <v>4168</v>
+        <v>5</v>
       </c>
       <c r="N33" s="0">
-        <v>55912</v>
+        <v>13863</v>
       </c>
       <c r="Q33" s="0">
         <v>0</v>
       </c>
       <c r="T33" s="0" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
       <c r="U33" s="0">
@@ -3026,13 +2949,13 @@
         <v>0</v>
       </c>
       <c r="W33" s="0">
-        <v>0.820278704166412</v>
+        <v>0.845360815525055</v>
       </c>
       <c r="X33" s="0">
-        <v>63081</v>
+        <v>16393</v>
       </c>
       <c r="AB33" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC33" s="0" t="inlineStr">
         <is>
@@ -3050,7 +2973,7 @@
         </is>
       </c>
       <c r="C34" s="1">
-        <v>45576</v>
+        <v>45566</v>
       </c>
       <c r="D34" s="0" t="inlineStr">
         <is>
@@ -3073,7 +2996,11 @@
       <c r="H34" s="0">
         <v>3</v>
       </c>
-      <c r="I34" s="0" t="inlineStr"/>
+      <c r="I34" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
       <c r="J34" s="0" t="inlineStr">
         <is>
           <t>Below Norm</t>
@@ -3085,23 +3012,20 @@
         </is>
       </c>
       <c r="L34" s="0">
-        <v>3049</v>
+        <v>6151</v>
       </c>
       <c r="M34" s="0">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="N34" s="0">
-        <v>3109</v>
-      </c>
-      <c r="O34" s="0">
-        <v>1</v>
+        <v>6173</v>
       </c>
       <c r="Q34" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T34" s="0" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
       <c r="U34" s="0">
@@ -3111,13 +3035,13 @@
         <v>0</v>
       </c>
       <c r="W34" s="0">
-        <v>0.861786305904388</v>
+        <v>0.84064507484436</v>
       </c>
       <c r="X34" s="0">
-        <v>3538</v>
+        <v>7317</v>
       </c>
       <c r="AB34" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC34" s="0" t="inlineStr">
         <is>
@@ -3135,7 +3059,7 @@
         </is>
       </c>
       <c r="C35" s="1">
-        <v>45576</v>
+        <v>45566</v>
       </c>
       <c r="D35" s="0" t="inlineStr">
         <is>
@@ -3158,7 +3082,11 @@
       <c r="H35" s="0">
         <v>3</v>
       </c>
-      <c r="I35" s="0" t="inlineStr"/>
+      <c r="I35" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
       <c r="J35" s="0" t="inlineStr">
         <is>
           <t>Below Norm</t>
@@ -3170,20 +3098,20 @@
         </is>
       </c>
       <c r="L35" s="0">
-        <v>1494</v>
+        <v>195</v>
       </c>
       <c r="N35" s="0">
-        <v>1494</v>
+        <v>195</v>
       </c>
       <c r="O35" s="0">
-        <v>173</v>
+        <v>20</v>
       </c>
       <c r="Q35" s="0">
-        <v>173</v>
+        <v>20</v>
       </c>
       <c r="T35" s="0" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
       <c r="U35" s="0">
@@ -3193,13 +3121,13 @@
         <v>0</v>
       </c>
       <c r="W35" s="0">
-        <v>0.862586617469788</v>
+        <v>0.840517222881317</v>
       </c>
       <c r="X35" s="0">
-        <v>1732</v>
+        <v>232</v>
       </c>
       <c r="AB35" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC35" s="0" t="inlineStr">
         <is>
@@ -3217,7 +3145,7 @@
         </is>
       </c>
       <c r="C36" s="1">
-        <v>45576</v>
+        <v>45566</v>
       </c>
       <c r="D36" s="0" t="inlineStr">
         <is>
@@ -3240,7 +3168,11 @@
       <c r="H36" s="0">
         <v>3</v>
       </c>
-      <c r="I36" s="0" t="inlineStr"/>
+      <c r="I36" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
       <c r="J36" s="0" t="inlineStr">
         <is>
           <t>Below Norm</t>
@@ -3251,6 +3183,9 @@
           <t>Pink</t>
         </is>
       </c>
+      <c r="L36" s="0">
+        <v>0</v>
+      </c>
       <c r="N36" s="0">
         <v>0</v>
       </c>
@@ -3261,7 +3196,7 @@
         <v>0</v>
       </c>
       <c r="AB36" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC36" s="0" t="inlineStr">
         <is>
@@ -3279,7 +3214,7 @@
         </is>
       </c>
       <c r="C37" s="1">
-        <v>45576</v>
+        <v>45566</v>
       </c>
       <c r="D37" s="0" t="inlineStr">
         <is>
@@ -3302,7 +3237,11 @@
       <c r="H37" s="0">
         <v>3</v>
       </c>
-      <c r="I37" s="0" t="inlineStr"/>
+      <c r="I37" s="0" t="inlineStr">
+        <is>
+          <t>3 - 5 m or to Bottom</t>
+        </is>
+      </c>
       <c r="J37" s="0" t="inlineStr">
         <is>
           <t>Below Norm</t>
@@ -3314,36 +3253,33 @@
         </is>
       </c>
       <c r="L37" s="0">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="N37" s="0">
-        <v>64</v>
-      </c>
-      <c r="O37" s="0">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="Q37" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T37" s="0" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
       <c r="U37" s="0">
-        <v>1</v>
+        <v>0.899999976158142</v>
       </c>
       <c r="V37" s="0">
         <v>0</v>
       </c>
       <c r="W37" s="0">
-        <v>0.853333353996277</v>
+        <v>0.531645596027374</v>
       </c>
       <c r="X37" s="0">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="AB37" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC37" s="0" t="inlineStr">
         <is>
@@ -3361,7 +3297,7 @@
         </is>
       </c>
       <c r="C38" s="1">
-        <v>45588</v>
+        <v>45576</v>
       </c>
       <c r="D38" s="0" t="inlineStr">
         <is>
@@ -3370,7 +3306,7 @@
       </c>
       <c r="E38" s="0" t="inlineStr">
         <is>
-          <t>heli</t>
+          <t>snrkl</t>
         </is>
       </c>
       <c r="F38" s="0" t="inlineStr">
@@ -3379,19 +3315,14 @@
         </is>
       </c>
       <c r="G38" s="0">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="H38" s="0">
-        <v>6</v>
-      </c>
-      <c r="I38" s="0" t="inlineStr">
-        <is>
-          <t>1 - 3 m</t>
-        </is>
+        <v>3</v>
       </c>
       <c r="J38" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K38" s="0" t="inlineStr">
@@ -3400,13 +3331,13 @@
         </is>
       </c>
       <c r="L38" s="0">
-        <v>99250</v>
+        <v>51744</v>
       </c>
       <c r="M38" s="0">
-        <v>3000</v>
+        <v>4168</v>
       </c>
       <c r="N38" s="0">
-        <v>102250</v>
+        <v>55912</v>
       </c>
       <c r="Q38" s="0">
         <v>0</v>
@@ -3423,13 +3354,13 @@
         <v>0</v>
       </c>
       <c r="W38" s="0">
-        <v>1</v>
+        <v>0.820278704166412</v>
       </c>
       <c r="X38" s="0">
-        <v>99250</v>
+        <v>63081</v>
       </c>
       <c r="AB38" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC38" s="0" t="inlineStr">
         <is>
@@ -3447,7 +3378,7 @@
         </is>
       </c>
       <c r="C39" s="1">
-        <v>45588</v>
+        <v>45576</v>
       </c>
       <c r="D39" s="0" t="inlineStr">
         <is>
@@ -3456,7 +3387,7 @@
       </c>
       <c r="E39" s="0" t="inlineStr">
         <is>
-          <t>heli</t>
+          <t>snrkl</t>
         </is>
       </c>
       <c r="F39" s="0" t="inlineStr">
@@ -3465,19 +3396,14 @@
         </is>
       </c>
       <c r="G39" s="0">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="H39" s="0">
-        <v>6</v>
-      </c>
-      <c r="I39" s="0" t="inlineStr">
-        <is>
-          <t>1 - 3 m</t>
-        </is>
+        <v>3</v>
       </c>
       <c r="J39" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K39" s="0" t="inlineStr">
@@ -3485,24 +3411,40 @@
           <t>Chinook</t>
         </is>
       </c>
-      <c r="L39" s="0"/>
-      <c r="M39" s="0"/>
+      <c r="L39" s="0">
+        <v>3049</v>
+      </c>
+      <c r="M39" s="0">
+        <v>60</v>
+      </c>
       <c r="N39" s="0">
-        <v>0</v>
-      </c>
-      <c r="O39" s="0"/>
+        <v>3109</v>
+      </c>
+      <c r="O39" s="0">
+        <v>1</v>
+      </c>
       <c r="Q39" s="0">
-        <v>0</v>
-      </c>
-      <c r="T39" s="0" t="inlineStr"/>
-      <c r="U39" s="0"/>
+        <v>1</v>
+      </c>
+      <c r="T39" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U39" s="0">
+        <v>1</v>
+      </c>
       <c r="V39" s="0">
         <v>0</v>
       </c>
-      <c r="W39" s="0"/>
-      <c r="X39" s="0"/>
+      <c r="W39" s="0">
+        <v>0.861786305904388</v>
+      </c>
+      <c r="X39" s="0">
+        <v>3538</v>
+      </c>
       <c r="AB39" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC39" s="0" t="inlineStr">
         <is>
@@ -3520,7 +3462,7 @@
         </is>
       </c>
       <c r="C40" s="1">
-        <v>45588</v>
+        <v>45576</v>
       </c>
       <c r="D40" s="0" t="inlineStr">
         <is>
@@ -3529,7 +3471,7 @@
       </c>
       <c r="E40" s="0" t="inlineStr">
         <is>
-          <t>heli</t>
+          <t>snrkl</t>
         </is>
       </c>
       <c r="F40" s="0" t="inlineStr">
@@ -3538,19 +3480,14 @@
         </is>
       </c>
       <c r="G40" s="0">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="H40" s="0">
-        <v>6</v>
-      </c>
-      <c r="I40" s="0" t="inlineStr">
-        <is>
-          <t>1 - 3 m</t>
-        </is>
+        <v>3</v>
       </c>
       <c r="J40" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K40" s="0" t="inlineStr">
@@ -3558,24 +3495,37 @@
           <t>Coho</t>
         </is>
       </c>
-      <c r="L40" s="0"/>
-      <c r="M40" s="0"/>
+      <c r="L40" s="0">
+        <v>1494</v>
+      </c>
       <c r="N40" s="0">
-        <v>0</v>
-      </c>
-      <c r="O40" s="0"/>
+        <v>1494</v>
+      </c>
+      <c r="O40" s="0">
+        <v>173</v>
+      </c>
       <c r="Q40" s="0">
-        <v>0</v>
-      </c>
-      <c r="T40" s="0" t="inlineStr"/>
-      <c r="U40" s="0"/>
+        <v>173</v>
+      </c>
+      <c r="T40" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U40" s="0">
+        <v>1</v>
+      </c>
       <c r="V40" s="0">
         <v>0</v>
       </c>
-      <c r="W40" s="0"/>
-      <c r="X40" s="0"/>
+      <c r="W40" s="0">
+        <v>0.862586617469788</v>
+      </c>
+      <c r="X40" s="0">
+        <v>1732</v>
+      </c>
       <c r="AB40" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC40" s="0" t="inlineStr">
         <is>
@@ -3593,7 +3543,7 @@
         </is>
       </c>
       <c r="C41" s="1">
-        <v>45588</v>
+        <v>45576</v>
       </c>
       <c r="D41" s="0" t="inlineStr">
         <is>
@@ -3602,7 +3552,7 @@
       </c>
       <c r="E41" s="0" t="inlineStr">
         <is>
-          <t>heli</t>
+          <t>snrkl</t>
         </is>
       </c>
       <c r="F41" s="0" t="inlineStr">
@@ -3611,19 +3561,14 @@
         </is>
       </c>
       <c r="G41" s="0">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="H41" s="0">
-        <v>6</v>
-      </c>
-      <c r="I41" s="0" t="inlineStr">
-        <is>
-          <t>1 - 3 m</t>
-        </is>
+        <v>3</v>
       </c>
       <c r="J41" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K41" s="0" t="inlineStr">
@@ -3631,6 +3576,9 @@
           <t>Pink</t>
         </is>
       </c>
+      <c r="L41" s="0">
+        <v>0</v>
+      </c>
       <c r="N41" s="0">
         <v>0</v>
       </c>
@@ -3641,7 +3589,7 @@
         <v>0</v>
       </c>
       <c r="AB41" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC41" s="0" t="inlineStr">
         <is>
@@ -3659,7 +3607,7 @@
         </is>
       </c>
       <c r="C42" s="1">
-        <v>45588</v>
+        <v>45576</v>
       </c>
       <c r="D42" s="0" t="inlineStr">
         <is>
@@ -3668,7 +3616,7 @@
       </c>
       <c r="E42" s="0" t="inlineStr">
         <is>
-          <t>heli</t>
+          <t>snrkl</t>
         </is>
       </c>
       <c r="F42" s="0" t="inlineStr">
@@ -3677,19 +3625,14 @@
         </is>
       </c>
       <c r="G42" s="0">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="H42" s="0">
-        <v>6</v>
-      </c>
-      <c r="I42" s="0" t="inlineStr">
-        <is>
-          <t>1 - 3 m</t>
-        </is>
+        <v>3</v>
       </c>
       <c r="J42" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Below Norm</t>
         </is>
       </c>
       <c r="K42" s="0" t="inlineStr">
@@ -3697,22 +3640,37 @@
           <t>Sockeye</t>
         </is>
       </c>
-      <c r="L42" s="0"/>
+      <c r="L42" s="0">
+        <v>64</v>
+      </c>
       <c r="N42" s="0">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="O42" s="0">
+        <v>1</v>
       </c>
       <c r="Q42" s="0">
-        <v>0</v>
-      </c>
-      <c r="T42" s="0" t="inlineStr"/>
-      <c r="U42" s="0"/>
+        <v>1</v>
+      </c>
+      <c r="T42" s="0" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+      <c r="U42" s="0">
+        <v>0.899999976158142</v>
+      </c>
       <c r="V42" s="0">
         <v>0</v>
       </c>
-      <c r="W42" s="0"/>
-      <c r="X42" s="0"/>
+      <c r="W42" s="0">
+        <v>0.853333353996277</v>
+      </c>
+      <c r="X42" s="0">
+        <v>83</v>
+      </c>
       <c r="AB42" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC42" s="0" t="inlineStr">
         <is>
@@ -3730,7 +3688,7 @@
         </is>
       </c>
       <c r="C43" s="1">
-        <v>45589</v>
+        <v>45588</v>
       </c>
       <c r="D43" s="0" t="inlineStr">
         <is>
@@ -3739,7 +3697,7 @@
       </c>
       <c r="E43" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F43" s="0" t="inlineStr">
@@ -3748,10 +3706,10 @@
         </is>
       </c>
       <c r="G43" s="0">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="H43" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I43" s="0" t="inlineStr">
         <is>
@@ -3760,7 +3718,7 @@
       </c>
       <c r="J43" s="0" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K43" s="0" t="inlineStr">
@@ -3769,20 +3727,20 @@
         </is>
       </c>
       <c r="L43" s="0">
-        <v>128669</v>
+        <v>99250</v>
       </c>
       <c r="M43" s="0">
-        <v>680</v>
+        <v>3000</v>
       </c>
       <c r="N43" s="0">
-        <v>129349</v>
+        <v>102250</v>
       </c>
       <c r="Q43" s="0">
         <v>0</v>
       </c>
       <c r="T43" s="0" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
       <c r="U43" s="0">
@@ -3792,13 +3750,13 @@
         <v>0</v>
       </c>
       <c r="W43" s="0">
-        <v>0.936926126480103</v>
+        <v>1</v>
       </c>
       <c r="X43" s="0">
-        <v>137331</v>
+        <v>99250</v>
       </c>
       <c r="AB43" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC43" s="0" t="inlineStr">
         <is>
@@ -3816,7 +3774,7 @@
         </is>
       </c>
       <c r="C44" s="1">
-        <v>45589</v>
+        <v>45588</v>
       </c>
       <c r="D44" s="0" t="inlineStr">
         <is>
@@ -3825,7 +3783,7 @@
       </c>
       <c r="E44" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F44" s="0" t="inlineStr">
@@ -3834,10 +3792,10 @@
         </is>
       </c>
       <c r="G44" s="0">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="H44" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I44" s="0" t="inlineStr">
         <is>
@@ -3846,7 +3804,7 @@
       </c>
       <c r="J44" s="0" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K44" s="0" t="inlineStr">
@@ -3855,37 +3813,19 @@
         </is>
       </c>
       <c r="L44" s="0">
-        <v>39</v>
-      </c>
-      <c r="M44" s="0"/>
+        <v>0</v>
+      </c>
       <c r="N44" s="0">
-        <v>39</v>
-      </c>
-      <c r="O44" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q44" s="0">
-        <v>1</v>
-      </c>
-      <c r="T44" s="0" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="U44" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V44" s="0">
         <v>0</v>
       </c>
-      <c r="W44" s="0">
-        <v>0.847826063632965</v>
-      </c>
-      <c r="X44" s="0">
-        <v>46</v>
-      </c>
       <c r="AB44" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC44" s="0" t="inlineStr">
         <is>
@@ -3903,7 +3843,7 @@
         </is>
       </c>
       <c r="C45" s="1">
-        <v>45589</v>
+        <v>45588</v>
       </c>
       <c r="D45" s="0" t="inlineStr">
         <is>
@@ -3912,7 +3852,7 @@
       </c>
       <c r="E45" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F45" s="0" t="inlineStr">
@@ -3921,10 +3861,10 @@
         </is>
       </c>
       <c r="G45" s="0">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="H45" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I45" s="0" t="inlineStr">
         <is>
@@ -3933,7 +3873,7 @@
       </c>
       <c r="J45" s="0" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K45" s="0" t="inlineStr">
@@ -3942,37 +3882,19 @@
         </is>
       </c>
       <c r="L45" s="0">
-        <v>21</v>
-      </c>
-      <c r="M45" s="0"/>
+        <v>0</v>
+      </c>
       <c r="N45" s="0">
-        <v>21</v>
-      </c>
-      <c r="O45" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q45" s="0">
-        <v>4</v>
-      </c>
-      <c r="T45" s="0" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="U45" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V45" s="0">
         <v>0</v>
       </c>
-      <c r="W45" s="0">
-        <v>0.91304349899292</v>
-      </c>
-      <c r="X45" s="0">
-        <v>23</v>
-      </c>
       <c r="AB45" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC45" s="0" t="inlineStr">
         <is>
@@ -3990,7 +3912,7 @@
         </is>
       </c>
       <c r="C46" s="1">
-        <v>45589</v>
+        <v>45588</v>
       </c>
       <c r="D46" s="0" t="inlineStr">
         <is>
@@ -3999,7 +3921,7 @@
       </c>
       <c r="E46" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F46" s="0" t="inlineStr">
@@ -4008,10 +3930,10 @@
         </is>
       </c>
       <c r="G46" s="0">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="H46" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I46" s="0" t="inlineStr">
         <is>
@@ -4020,7 +3942,7 @@
       </c>
       <c r="J46" s="0" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K46" s="0" t="inlineStr">
@@ -4028,6 +3950,9 @@
           <t>Pink</t>
         </is>
       </c>
+      <c r="L46" s="0">
+        <v>0</v>
+      </c>
       <c r="N46" s="0">
         <v>0</v>
       </c>
@@ -4038,7 +3963,7 @@
         <v>0</v>
       </c>
       <c r="AB46" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC46" s="0" t="inlineStr">
         <is>
@@ -4056,7 +3981,7 @@
         </is>
       </c>
       <c r="C47" s="1">
-        <v>45589</v>
+        <v>45588</v>
       </c>
       <c r="D47" s="0" t="inlineStr">
         <is>
@@ -4065,7 +3990,7 @@
       </c>
       <c r="E47" s="0" t="inlineStr">
         <is>
-          <t>snrkl</t>
+          <t>heli</t>
         </is>
       </c>
       <c r="F47" s="0" t="inlineStr">
@@ -4074,10 +3999,10 @@
         </is>
       </c>
       <c r="G47" s="0">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="H47" s="0">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I47" s="0" t="inlineStr">
         <is>
@@ -4086,7 +4011,7 @@
       </c>
       <c r="J47" s="0" t="inlineStr">
         <is>
-          <t>Flood</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="K47" s="0" t="inlineStr">
@@ -4095,33 +4020,19 @@
         </is>
       </c>
       <c r="L47" s="0">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N47" s="0">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q47" s="0">
         <v>0</v>
       </c>
-      <c r="T47" s="0" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="U47" s="0">
-        <v>1</v>
-      </c>
       <c r="V47" s="0">
         <v>0</v>
       </c>
-      <c r="W47" s="0">
-        <v>1</v>
-      </c>
-      <c r="X47" s="0">
-        <v>2</v>
-      </c>
       <c r="AB47" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC47" s="0" t="inlineStr">
         <is>
@@ -4139,7 +4050,7 @@
         </is>
       </c>
       <c r="C48" s="1">
-        <v>45603</v>
+        <v>45589</v>
       </c>
       <c r="D48" s="0" t="inlineStr">
         <is>
@@ -4178,13 +4089,13 @@
         </is>
       </c>
       <c r="L48" s="0">
-        <v>493</v>
+        <v>29419</v>
       </c>
       <c r="M48" s="0">
-        <v>2388</v>
+        <v>680</v>
       </c>
       <c r="N48" s="0">
-        <v>2881</v>
+        <v>30099</v>
       </c>
       <c r="Q48" s="0">
         <v>0</v>
@@ -4195,19 +4106,19 @@
         </is>
       </c>
       <c r="U48" s="0">
-        <v>1</v>
+        <v>0.850000023841858</v>
       </c>
       <c r="V48" s="0">
         <v>0</v>
       </c>
       <c r="W48" s="0">
-        <v>0.767912745475769</v>
+        <v>0.772537469863892</v>
       </c>
       <c r="X48" s="0">
-        <v>642</v>
+        <v>44801</v>
       </c>
       <c r="AB48" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC48" s="0" t="inlineStr">
         <is>
@@ -4225,7 +4136,7 @@
         </is>
       </c>
       <c r="C49" s="1">
-        <v>45603</v>
+        <v>45589</v>
       </c>
       <c r="D49" s="0" t="inlineStr">
         <is>
@@ -4264,19 +4175,16 @@
         </is>
       </c>
       <c r="L49" s="0">
-        <v>4</v>
-      </c>
-      <c r="M49" s="0">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="N49" s="0">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="O49" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q49" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T49" s="0" t="inlineStr">
         <is>
@@ -4284,19 +4192,19 @@
         </is>
       </c>
       <c r="U49" s="0">
-        <v>1</v>
+        <v>0.800000011920929</v>
       </c>
       <c r="V49" s="0">
         <v>0</v>
       </c>
       <c r="W49" s="0">
-        <v>0.800000011920929</v>
+        <v>0.847826063632965</v>
       </c>
       <c r="X49" s="0">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="AB49" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC49" s="0" t="inlineStr">
         <is>
@@ -4314,7 +4222,7 @@
         </is>
       </c>
       <c r="C50" s="1">
-        <v>45603</v>
+        <v>45589</v>
       </c>
       <c r="D50" s="0" t="inlineStr">
         <is>
@@ -4353,39 +4261,36 @@
         </is>
       </c>
       <c r="L50" s="0">
-        <v>1302</v>
-      </c>
-      <c r="M50" s="0">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="N50" s="0">
-        <v>1310</v>
+        <v>21</v>
       </c>
       <c r="O50" s="0">
-        <v>148</v>
+        <v>4</v>
       </c>
       <c r="Q50" s="0">
-        <v>148</v>
+        <v>4</v>
       </c>
       <c r="T50" s="0" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>L</t>
         </is>
       </c>
       <c r="U50" s="0">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="V50" s="0">
         <v>0</v>
       </c>
       <c r="W50" s="0">
-        <v>0.810709834098816</v>
+        <v>0.91304349899292</v>
       </c>
       <c r="X50" s="0">
-        <v>1606</v>
+        <v>46</v>
       </c>
       <c r="AB50" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC50" s="0" t="inlineStr">
         <is>
@@ -4403,7 +4308,7 @@
         </is>
       </c>
       <c r="C51" s="1">
-        <v>45603</v>
+        <v>45589</v>
       </c>
       <c r="D51" s="0" t="inlineStr">
         <is>
@@ -4441,6 +4346,9 @@
           <t>Pink</t>
         </is>
       </c>
+      <c r="L51" s="0">
+        <v>0</v>
+      </c>
       <c r="N51" s="0">
         <v>0</v>
       </c>
@@ -4451,7 +4359,7 @@
         <v>0</v>
       </c>
       <c r="AB51" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC51" s="0" t="inlineStr">
         <is>
@@ -4469,7 +4377,7 @@
         </is>
       </c>
       <c r="C52" s="1">
-        <v>45603</v>
+        <v>45589</v>
       </c>
       <c r="D52" s="0" t="inlineStr">
         <is>
@@ -4507,17 +4415,34 @@
           <t>Sockeye</t>
         </is>
       </c>
+      <c r="L52" s="0">
+        <v>2</v>
+      </c>
       <c r="N52" s="0">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q52" s="0">
         <v>0</v>
       </c>
+      <c r="T52" s="0" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="U52" s="0">
+        <v>0.5</v>
+      </c>
       <c r="V52" s="0">
         <v>0</v>
       </c>
+      <c r="W52" s="0">
+        <v>1</v>
+      </c>
+      <c r="X52" s="0">
+        <v>4</v>
+      </c>
       <c r="AB52" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC52" s="0" t="inlineStr">
         <is>
@@ -4535,7 +4460,7 @@
         </is>
       </c>
       <c r="C53" s="1">
-        <v>45609</v>
+        <v>45603</v>
       </c>
       <c r="D53" s="0" t="inlineStr">
         <is>
@@ -4558,10 +4483,14 @@
       <c r="H53" s="0">
         <v>3</v>
       </c>
-      <c r="I53" s="0" t="inlineStr"/>
+      <c r="I53" s="0" t="inlineStr">
+        <is>
+          <t>1 - 3 m</t>
+        </is>
+      </c>
       <c r="J53" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Flood</t>
         </is>
       </c>
       <c r="K53" s="0" t="inlineStr">
@@ -4570,25 +4499,36 @@
         </is>
       </c>
       <c r="L53" s="0">
-        <v>59</v>
+        <v>493</v>
       </c>
       <c r="M53" s="0">
-        <v>0</v>
+        <v>2388</v>
       </c>
       <c r="N53" s="0">
-        <v>59</v>
+        <v>2881</v>
       </c>
       <c r="Q53" s="0">
         <v>0</v>
       </c>
+      <c r="T53" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U53" s="0">
+        <v>1</v>
+      </c>
       <c r="V53" s="0">
         <v>0</v>
       </c>
       <c r="W53" s="0">
-        <v>0.830985903739929</v>
+        <v>0.767912745475769</v>
+      </c>
+      <c r="X53" s="0">
+        <v>642</v>
       </c>
       <c r="AB53" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC53" s="0" t="inlineStr">
         <is>
@@ -4606,7 +4546,7 @@
         </is>
       </c>
       <c r="C54" s="1">
-        <v>45609</v>
+        <v>45603</v>
       </c>
       <c r="D54" s="0" t="inlineStr">
         <is>
@@ -4629,10 +4569,14 @@
       <c r="H54" s="0">
         <v>3</v>
       </c>
-      <c r="I54" s="0" t="inlineStr"/>
+      <c r="I54" s="0" t="inlineStr">
+        <is>
+          <t>1 - 3 m</t>
+        </is>
+      </c>
       <c r="J54" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Flood</t>
         </is>
       </c>
       <c r="K54" s="0" t="inlineStr">
@@ -4655,14 +4599,25 @@
       <c r="Q54" s="0">
         <v>0</v>
       </c>
+      <c r="T54" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U54" s="0">
+        <v>1</v>
+      </c>
       <c r="V54" s="0">
         <v>0</v>
       </c>
       <c r="W54" s="0">
         <v>0.800000011920929</v>
       </c>
+      <c r="X54" s="0">
+        <v>5</v>
+      </c>
       <c r="AB54" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC54" s="0" t="inlineStr">
         <is>
@@ -4680,7 +4635,7 @@
         </is>
       </c>
       <c r="C55" s="1">
-        <v>45609</v>
+        <v>45603</v>
       </c>
       <c r="D55" s="0" t="inlineStr">
         <is>
@@ -4703,10 +4658,14 @@
       <c r="H55" s="0">
         <v>3</v>
       </c>
-      <c r="I55" s="0" t="inlineStr"/>
+      <c r="I55" s="0" t="inlineStr">
+        <is>
+          <t>1 - 3 m</t>
+        </is>
+      </c>
       <c r="J55" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Flood</t>
         </is>
       </c>
       <c r="K55" s="0" t="inlineStr">
@@ -4715,28 +4674,39 @@
         </is>
       </c>
       <c r="L55" s="0">
-        <v>626</v>
+        <v>1302</v>
       </c>
       <c r="M55" s="0">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="N55" s="0">
-        <v>627</v>
+        <v>1310</v>
       </c>
       <c r="O55" s="0">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="Q55" s="0">
-        <v>100</v>
+        <v>148</v>
+      </c>
+      <c r="T55" s="0" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="U55" s="0">
+        <v>0.899999976158142</v>
       </c>
       <c r="V55" s="0">
         <v>0</v>
       </c>
       <c r="W55" s="0">
-        <v>1</v>
+        <v>0.810709834098816</v>
+      </c>
+      <c r="X55" s="0">
+        <v>1784</v>
       </c>
       <c r="AB55" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC55" s="0" t="inlineStr">
         <is>
@@ -4754,7 +4724,7 @@
         </is>
       </c>
       <c r="C56" s="1">
-        <v>45609</v>
+        <v>45603</v>
       </c>
       <c r="D56" s="0" t="inlineStr">
         <is>
@@ -4777,10 +4747,14 @@
       <c r="H56" s="0">
         <v>3</v>
       </c>
-      <c r="I56" s="0" t="inlineStr"/>
+      <c r="I56" s="0" t="inlineStr">
+        <is>
+          <t>1 - 3 m</t>
+        </is>
+      </c>
       <c r="J56" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Flood</t>
         </is>
       </c>
       <c r="K56" s="0" t="inlineStr">
@@ -4788,6 +4762,9 @@
           <t>Pink</t>
         </is>
       </c>
+      <c r="L56" s="0">
+        <v>0</v>
+      </c>
       <c r="N56" s="0">
         <v>0</v>
       </c>
@@ -4798,7 +4775,7 @@
         <v>0</v>
       </c>
       <c r="AB56" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC56" s="0" t="inlineStr">
         <is>
@@ -4816,7 +4793,7 @@
         </is>
       </c>
       <c r="C57" s="1">
-        <v>45609</v>
+        <v>45603</v>
       </c>
       <c r="D57" s="0" t="inlineStr">
         <is>
@@ -4839,10 +4816,14 @@
       <c r="H57" s="0">
         <v>3</v>
       </c>
-      <c r="I57" s="0" t="inlineStr"/>
+      <c r="I57" s="0" t="inlineStr">
+        <is>
+          <t>1 - 3 m</t>
+        </is>
+      </c>
       <c r="J57" s="0" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Flood</t>
         </is>
       </c>
       <c r="K57" s="0" t="inlineStr">
@@ -4850,17 +4831,26 @@
           <t>Sockeye</t>
         </is>
       </c>
+      <c r="L57" s="0">
+        <v>0</v>
+      </c>
       <c r="N57" s="0">
         <v>0</v>
       </c>
       <c r="Q57" s="0">
         <v>0</v>
       </c>
+      <c r="U57" s="0">
+        <v>1</v>
+      </c>
       <c r="V57" s="0">
         <v>0</v>
       </c>
+      <c r="X57" s="0">
+        <v>0</v>
+      </c>
       <c r="AB57" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC57" s="0" t="inlineStr">
         <is>
@@ -4943,7 +4933,7 @@
         <v>478</v>
       </c>
       <c r="AB58" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC58" s="0" t="inlineStr">
         <is>
@@ -5009,7 +4999,7 @@
         <v>0</v>
       </c>
       <c r="AB59" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC59" s="0" t="inlineStr">
         <is>
@@ -5075,7 +5065,7 @@
         <v>0</v>
       </c>
       <c r="AB60" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC60" s="0" t="inlineStr">
         <is>
@@ -5141,7 +5131,7 @@
         <v>0</v>
       </c>
       <c r="AB61" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC61" s="0" t="inlineStr">
         <is>
@@ -5207,7 +5197,7 @@
         <v>0</v>
       </c>
       <c r="AB62" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC62" s="0" t="inlineStr">
         <is>
@@ -5282,7 +5272,7 @@
         <v>0.899999976158142</v>
       </c>
       <c r="AB63" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC63" s="0" t="inlineStr">
         <is>
@@ -5348,7 +5338,7 @@
         <v>0</v>
       </c>
       <c r="AB64" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC64" s="0" t="inlineStr">
         <is>
@@ -5426,7 +5416,7 @@
         <v>0.899999976158142</v>
       </c>
       <c r="AB65" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC65" s="0" t="inlineStr">
         <is>
@@ -5492,7 +5482,7 @@
         <v>0</v>
       </c>
       <c r="AB66" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC66" s="0" t="inlineStr">
         <is>
@@ -5558,7 +5548,7 @@
         <v>0</v>
       </c>
       <c r="AB67" s="1">
-        <v>45624.412349537</v>
+        <v>45630.6763888889</v>
       </c>
       <c r="AC67" s="0" t="inlineStr">
         <is>

</xml_diff>